<commit_message>
- added bootloader specifications
</commit_message>
<xml_diff>
--- a/doc/Bootloader_Interface_Specifications.xlsx
+++ b/doc/Bootloader_Interface_Specifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\ORDERBOB_ECS__2023\SOFTWARE\MASTER_SOURCE\ECS_Bootloader\OrderBob\middleware\boot\boot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB77B6C4-1C50-4B85-8D71-E1ACEAFCD5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8A9C65-4419-4423-8FF1-493E0493E2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -958,12 +958,6 @@
     </r>
   </si>
   <si>
-    <t>Connect to bootlaoder command</t>
-  </si>
-  <si>
-    <t>Connect to bootlaoder response command</t>
-  </si>
-  <si>
     <t>0x2B</t>
   </si>
   <si>
@@ -989,6 +983,12 @@
   </si>
   <si>
     <t>0x11</t>
+  </si>
+  <si>
+    <t>Connect to bootloader command</t>
+  </si>
+  <si>
+    <t>Connect to bootloader response command</t>
   </si>
 </sst>
 </file>
@@ -1136,14 +1136,13 @@
       <b/>
       <i/>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1216,6 +1215,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -1560,111 +1565,162 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1672,14 +1728,8 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1687,23 +1737,11 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1713,52 +1751,22 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2055,171 +2063,177 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="12"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="12"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="12"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -2228,12 +2242,6 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2244,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC1FC0B-6045-46A4-BC27-706096C9D78D}">
   <dimension ref="A4:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,507 +2262,507 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="10">
         <v>2</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="10">
         <v>3</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="10">
         <v>4</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="10">
         <v>5</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="10">
         <v>6</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="10">
         <v>7</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="10">
         <v>8</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="10">
         <v>9</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="10">
         <v>10</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="10">
         <v>11</v>
       </c>
-      <c r="O6" s="26" t="s">
+      <c r="O6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="28"/>
-      <c r="C7" s="29" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30" t="s">
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="31"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="74"/>
     </row>
     <row r="11" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="33"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="14">
         <v>0</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="14">
         <v>1</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="14">
         <v>2</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="14">
         <v>3</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="14">
         <v>4</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="14">
         <v>5</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="14">
         <v>6</v>
       </c>
-      <c r="J13" s="35">
+      <c r="J13" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="37" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="38"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="60" t="s">
+      <c r="D15" s="45"/>
+      <c r="E15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="66" t="s">
+      <c r="F15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="68" t="s">
+      <c r="H15" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="68"/>
-      <c r="J15" s="61" t="s">
+      <c r="I15" s="46"/>
+      <c r="J15" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="69" t="s">
+      <c r="H16" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="69" t="s">
+      <c r="I16" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="62" t="s">
+      <c r="J16" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58" t="s">
+      <c r="C18" s="68"/>
+      <c r="D18" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="59"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="70"/>
     </row>
     <row r="19" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45" t="s">
+      <c r="C19" s="61"/>
+      <c r="D19" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="47"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:25" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="50" t="s">
+      <c r="C20" s="61"/>
+      <c r="D20" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="49"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="64"/>
     </row>
     <row r="21" spans="1:25" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="44"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="66"/>
     </row>
     <row r="22" spans="1:25" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="50" t="s">
+      <c r="C22" s="61"/>
+      <c r="D22" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="49"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="64"/>
     </row>
     <row r="23" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="72" t="s">
+      <c r="C23" s="59"/>
+      <c r="D23" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="47"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="57"/>
     </row>
     <row r="24" spans="1:25" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="73" t="s">
+      <c r="C24" s="51"/>
+      <c r="D24" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
     </row>
     <row r="27" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="33"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="49"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="49"/>
     </row>
     <row r="28" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="34">
+      <c r="C29" s="14">
         <v>0</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="14">
         <v>1</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="14">
         <v>2</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="14">
         <v>3</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="14">
         <v>4</v>
       </c>
-      <c r="H29" s="34">
+      <c r="H29" s="14">
         <v>5</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="14">
         <v>6</v>
       </c>
-      <c r="J29" s="35">
+      <c r="J29" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="37" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="60" t="s">
+      <c r="D31" s="45"/>
+      <c r="E31" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="66" t="s">
+      <c r="F31" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="68" t="s">
+      <c r="H31" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I31" s="68"/>
-      <c r="J31" s="61" t="s">
+      <c r="I31" s="46"/>
+      <c r="J31" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="41" t="s">
+      <c r="E32" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="67" t="s">
+      <c r="H32" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="42" t="s">
+    </row>
+    <row r="36" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A36" s="13"/>
+      <c r="B36" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="49"/>
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="49"/>
+    </row>
+    <row r="38" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="L38" s="75" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="32"/>
-      <c r="B36" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="33"/>
-      <c r="S36" s="33"/>
-      <c r="T36" s="33"/>
-      <c r="U36" s="33"/>
-      <c r="V36" s="33"/>
-      <c r="W36" s="33"/>
-      <c r="X36" s="33"/>
-      <c r="Y36" s="33"/>
-    </row>
-    <row r="38" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
-      <c r="L38" s="75" t="s">
-        <v>47</v>
       </c>
       <c r="M38" s="75"/>
       <c r="N38" s="75"/>
@@ -2766,204 +2774,196 @@
       <c r="T38" s="75"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C39" s="14">
         <v>0</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="14">
         <v>1</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="14">
         <v>2</v>
       </c>
-      <c r="F39" s="34">
+      <c r="F39" s="14">
         <v>3</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="14">
         <v>4</v>
       </c>
-      <c r="H39" s="34">
+      <c r="H39" s="14">
         <v>5</v>
       </c>
-      <c r="I39" s="34">
+      <c r="I39" s="14">
         <v>6</v>
       </c>
-      <c r="J39" s="35">
+      <c r="J39" s="15">
         <v>7</v>
       </c>
-      <c r="L39" s="25" t="s">
+      <c r="L39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M39" s="34">
+      <c r="M39" s="14">
         <v>0</v>
       </c>
-      <c r="N39" s="34">
+      <c r="N39" s="14">
         <v>1</v>
       </c>
-      <c r="O39" s="34">
+      <c r="O39" s="14">
         <v>2</v>
       </c>
-      <c r="P39" s="34">
+      <c r="P39" s="14">
         <v>3</v>
       </c>
-      <c r="Q39" s="34">
+      <c r="Q39" s="14">
         <v>4</v>
       </c>
-      <c r="R39" s="34">
+      <c r="R39" s="14">
         <v>5</v>
       </c>
-      <c r="S39" s="34">
+      <c r="S39" s="14">
         <v>6</v>
       </c>
-      <c r="T39" s="35">
+      <c r="T39" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="36"/>
-      <c r="C40" s="37" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="38"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="37" t="s">
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="48"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="N40" s="37"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="37"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="38"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="47"/>
+      <c r="Q40" s="47"/>
+      <c r="R40" s="47"/>
+      <c r="S40" s="47"/>
+      <c r="T40" s="48"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="64"/>
-      <c r="E41" s="60" t="s">
+      <c r="D41" s="45"/>
+      <c r="E41" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="66" t="s">
+      <c r="F41" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G41" s="39" t="s">
+      <c r="G41" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H41" s="68" t="s">
+      <c r="H41" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I41" s="68"/>
-      <c r="J41" s="61" t="s">
+      <c r="I41" s="46"/>
+      <c r="J41" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="L41" s="36" t="s">
+      <c r="L41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="M41" s="63" t="s">
+      <c r="M41" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="N41" s="64"/>
-      <c r="O41" s="60" t="s">
+      <c r="N41" s="45"/>
+      <c r="O41" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P41" s="66" t="s">
+      <c r="P41" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="Q41" s="39" t="s">
+      <c r="Q41" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R41" s="68" t="s">
+      <c r="R41" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="S41" s="68"/>
-      <c r="T41" s="61" t="s">
+      <c r="S41" s="46"/>
+      <c r="T41" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="H42" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="I42" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="J42" s="74" t="s">
+      <c r="E42" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J42" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="L42" s="28" t="s">
+      <c r="L42" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M42" s="40" t="s">
+      <c r="M42" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N42" s="40" t="s">
+      <c r="N42" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="O42" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="P42" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q42" s="42" t="s">
+      <c r="O42" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="P42" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="R42" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="S42" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="T42" s="74" t="s">
+      <c r="Q42" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="R42" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="S42" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="T42" s="27" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="L38:T38"/>
-    <mergeCell ref="M40:T40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="R41:S41"/>
-    <mergeCell ref="B27:Y27"/>
-    <mergeCell ref="B36:Y36"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="K7:P7"/>
+    <mergeCell ref="B11:Y11"/>
+    <mergeCell ref="C14:J14"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:J24"/>
     <mergeCell ref="C15:D15"/>
@@ -2980,11 +2980,19 @@
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D19:J19"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="K7:P7"/>
-    <mergeCell ref="B11:Y11"/>
-    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B27:Y27"/>
+    <mergeCell ref="B36:Y36"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="L38:T38"/>
+    <mergeCell ref="M40:T40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="C40:J40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- updated bootloader interface specs
</commit_message>
<xml_diff>
--- a/doc/Bootloader_Interface_Specifications.xlsx
+++ b/doc/Bootloader_Interface_Specifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\ORDERBOB_ECS__2023\SOFTWARE\MASTER_SOURCE\ECS_Bootloader\OrderBob\middleware\boot\boot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1130E0B4-8364-4CCB-A6E5-4D80EE8D483B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D333D8DD-7745-41BF-BAC1-957018BFFF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1354,7 +1354,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-TODO: Specify how to calculate CRC</t>
+TODO: Specify how to calculate CRC. CRC ALGO MUST RETURN NON-ZERO VALUE IF ALL ZERO VALUES ARE INSERTED!!!!</t>
     </r>
   </si>
 </sst>
@@ -2066,25 +2066,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2103,6 +2091,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2111,11 +2192,47 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2123,128 +2240,11 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2667,19 +2667,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2692,14 +2692,14 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -2711,20 +2711,20 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="48"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="37"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
       <c r="H6" s="38"/>
@@ -2735,7 +2735,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="43"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
@@ -2746,7 +2746,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="37"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
@@ -2757,7 +2757,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="37"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
@@ -2768,7 +2768,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="37"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
@@ -2779,7 +2779,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="37"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
@@ -2790,7 +2790,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="37"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
@@ -2801,7 +2801,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="37"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
@@ -2812,7 +2812,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="37"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
@@ -2823,21 +2823,15 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="42"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -2846,6 +2840,12 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2856,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC1FC0B-6045-46A4-BC27-706096C9D78D}">
   <dimension ref="A2:Y115"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AD22" sqref="AD22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2867,32 +2867,32 @@
   <sheetData>
     <row r="2" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -2944,53 +2944,53 @@
     </row>
     <row r="5" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
-      <c r="C5" s="99" t="s">
+      <c r="C5" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="100" t="s">
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="101"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="56"/>
     </row>
     <row r="7" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="31"/>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="71"/>
-      <c r="Y7" s="71"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="53"/>
+      <c r="Y7" s="53"/>
     </row>
     <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -3024,25 +3024,25 @@
     </row>
     <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="67"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="20" t="s">
         <v>23</v>
       </c>
@@ -3052,10 +3052,10 @@
       <c r="G11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="70" t="s">
+      <c r="H11" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="70"/>
+      <c r="I11" s="61"/>
       <c r="J11" s="21" t="s">
         <v>34</v>
       </c>
@@ -3091,138 +3091,138 @@
     </row>
     <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55" t="s">
+      <c r="C14" s="81"/>
+      <c r="D14" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="56"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="83"/>
     </row>
     <row r="15" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="98" t="s">
+      <c r="C15" s="73"/>
+      <c r="D15" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="89"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="69"/>
     </row>
     <row r="16" spans="1:25" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="92" t="s">
+      <c r="C16" s="73"/>
+      <c r="D16" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="94"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="76"/>
     </row>
     <row r="17" spans="1:25" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="95" t="s">
+      <c r="C17" s="73"/>
+      <c r="D17" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="96"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="78"/>
     </row>
     <row r="18" spans="1:25" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="97" t="s">
+      <c r="C18" s="73"/>
+      <c r="D18" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="94"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="76"/>
     </row>
     <row r="19" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="87" t="s">
+      <c r="C19" s="71"/>
+      <c r="D19" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="89"/>
-    </row>
-    <row r="20" spans="1:25" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="61" t="s">
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="69"/>
+    </row>
+    <row r="20" spans="1:25" ht="231" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="84" t="s">
+      <c r="C20" s="63"/>
+      <c r="D20" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="86"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="66"/>
     </row>
     <row r="23" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="31"/>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="71"/>
-      <c r="O23" s="71"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="71"/>
-      <c r="U23" s="71"/>
-      <c r="V23" s="71"/>
-      <c r="W23" s="71"/>
-      <c r="X23" s="71"/>
-      <c r="Y23" s="71"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+      <c r="Y23" s="53"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -3256,25 +3256,25 @@
     </row>
     <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="67"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="68" t="s">
+      <c r="C27" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="69"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="20" t="s">
         <v>23</v>
       </c>
@@ -3284,10 +3284,10 @@
       <c r="G27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="70" t="s">
+      <c r="H27" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="70"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="21" t="s">
         <v>34</v>
       </c>
@@ -3326,129 +3326,129 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55" t="s">
+      <c r="C31" s="81"/>
+      <c r="D31" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="55"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="56"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="82"/>
+      <c r="Q31" s="82"/>
+      <c r="R31" s="82"/>
+      <c r="S31" s="83"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59" t="s">
+      <c r="C32" s="73"/>
+      <c r="D32" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="59"/>
-      <c r="N32" s="59"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="60"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="98"/>
+      <c r="N32" s="98"/>
+      <c r="O32" s="98"/>
+      <c r="P32" s="98"/>
+      <c r="Q32" s="98"/>
+      <c r="R32" s="98"/>
+      <c r="S32" s="99"/>
     </row>
     <row r="33" spans="1:25" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="63" t="s">
+      <c r="C33" s="63"/>
+      <c r="D33" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="64"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="100"/>
+      <c r="Q33" s="100"/>
+      <c r="R33" s="100"/>
+      <c r="S33" s="101"/>
     </row>
     <row r="35" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A35" s="31"/>
-      <c r="B35" s="71" t="s">
+      <c r="B35" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="71"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="71"/>
-      <c r="O35" s="71"/>
-      <c r="P35" s="71"/>
-      <c r="Q35" s="71"/>
-      <c r="R35" s="71"/>
-      <c r="S35" s="71"/>
-      <c r="T35" s="71"/>
-      <c r="U35" s="71"/>
-      <c r="V35" s="71"/>
-      <c r="W35" s="71"/>
-      <c r="X35" s="71"/>
-      <c r="Y35" s="71"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="53"/>
+      <c r="T35" s="53"/>
+      <c r="U35" s="53"/>
+      <c r="V35" s="53"/>
+      <c r="W35" s="53"/>
+      <c r="X35" s="53"/>
+      <c r="Y35" s="53"/>
     </row>
     <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="65"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="L37" s="72" t="s">
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="L37" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
-      <c r="O37" s="72"/>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
+      <c r="M37" s="86"/>
+      <c r="N37" s="86"/>
+      <c r="O37" s="86"/>
+      <c r="P37" s="86"/>
+      <c r="Q37" s="86"/>
+      <c r="R37" s="86"/>
+      <c r="S37" s="86"/>
+      <c r="T37" s="86"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
@@ -3508,36 +3508,36 @@
     </row>
     <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="15"/>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="67"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="58"/>
       <c r="L39" s="15"/>
-      <c r="M39" s="66" t="s">
+      <c r="M39" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="N39" s="66"/>
-      <c r="O39" s="66"/>
-      <c r="P39" s="66"/>
-      <c r="Q39" s="66"/>
-      <c r="R39" s="66"/>
-      <c r="S39" s="66"/>
-      <c r="T39" s="67"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="57"/>
+      <c r="P39" s="57"/>
+      <c r="Q39" s="57"/>
+      <c r="R39" s="57"/>
+      <c r="S39" s="57"/>
+      <c r="T39" s="58"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="69"/>
+      <c r="D40" s="60"/>
       <c r="E40" s="20" t="s">
         <v>23</v>
       </c>
@@ -3547,20 +3547,20 @@
       <c r="G40" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H40" s="70" t="s">
+      <c r="H40" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="70"/>
+      <c r="I40" s="61"/>
       <c r="J40" s="21" t="s">
         <v>34</v>
       </c>
       <c r="L40" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M40" s="68" t="s">
+      <c r="M40" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="N40" s="69"/>
+      <c r="N40" s="60"/>
       <c r="O40" s="20" t="s">
         <v>23</v>
       </c>
@@ -3570,10 +3570,10 @@
       <c r="Q40" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="R40" s="70" t="s">
+      <c r="R40" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="S40" s="70"/>
+      <c r="S40" s="61"/>
       <c r="T40" s="21" t="s">
         <v>34</v>
       </c>
@@ -3636,105 +3636,105 @@
     </row>
     <row r="42" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="54"/>
-      <c r="D43" s="55" t="s">
+      <c r="C43" s="81"/>
+      <c r="D43" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
-      <c r="N43" s="55"/>
-      <c r="O43" s="55"/>
-      <c r="P43" s="55"/>
-      <c r="Q43" s="55"/>
-      <c r="R43" s="55"/>
-      <c r="S43" s="56"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="82"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="82"/>
+      <c r="I43" s="82"/>
+      <c r="J43" s="82"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="82"/>
+      <c r="N43" s="82"/>
+      <c r="O43" s="82"/>
+      <c r="P43" s="82"/>
+      <c r="Q43" s="82"/>
+      <c r="R43" s="82"/>
+      <c r="S43" s="83"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="58"/>
-      <c r="D44" s="59" t="s">
+      <c r="C44" s="73"/>
+      <c r="D44" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
-      <c r="L44" s="59"/>
-      <c r="M44" s="59"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="59"/>
-      <c r="Q44" s="59"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="60"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="98"/>
+      <c r="H44" s="98"/>
+      <c r="I44" s="98"/>
+      <c r="J44" s="98"/>
+      <c r="K44" s="98"/>
+      <c r="L44" s="98"/>
+      <c r="M44" s="98"/>
+      <c r="N44" s="98"/>
+      <c r="O44" s="98"/>
+      <c r="P44" s="98"/>
+      <c r="Q44" s="98"/>
+      <c r="R44" s="98"/>
+      <c r="S44" s="99"/>
     </row>
     <row r="45" spans="1:25" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="62"/>
-      <c r="D45" s="63" t="s">
+      <c r="C45" s="63"/>
+      <c r="D45" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="63"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="63"/>
-      <c r="R45" s="63"/>
-      <c r="S45" s="64"/>
+      <c r="E45" s="100"/>
+      <c r="F45" s="100"/>
+      <c r="G45" s="100"/>
+      <c r="H45" s="100"/>
+      <c r="I45" s="100"/>
+      <c r="J45" s="100"/>
+      <c r="K45" s="100"/>
+      <c r="L45" s="100"/>
+      <c r="M45" s="100"/>
+      <c r="N45" s="100"/>
+      <c r="O45" s="100"/>
+      <c r="P45" s="100"/>
+      <c r="Q45" s="100"/>
+      <c r="R45" s="100"/>
+      <c r="S45" s="101"/>
     </row>
     <row r="48" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A48" s="31"/>
-      <c r="B48" s="71" t="s">
+      <c r="B48" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="71"/>
-      <c r="I48" s="71"/>
-      <c r="J48" s="71"/>
-      <c r="K48" s="71"/>
-      <c r="L48" s="71"/>
-      <c r="M48" s="71"/>
-      <c r="N48" s="71"/>
-      <c r="O48" s="71"/>
-      <c r="P48" s="71"/>
-      <c r="Q48" s="71"/>
-      <c r="R48" s="71"/>
-      <c r="S48" s="71"/>
-      <c r="T48" s="71"/>
-      <c r="U48" s="71"/>
-      <c r="V48" s="71"/>
-      <c r="W48" s="71"/>
-      <c r="X48" s="71"/>
-      <c r="Y48" s="71"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="53"/>
+      <c r="T48" s="53"/>
+      <c r="U48" s="53"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="53"/>
+      <c r="X48" s="53"/>
+      <c r="Y48" s="53"/>
     </row>
     <row r="49" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
@@ -3804,39 +3804,39 @@
     </row>
     <row r="51" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="15"/>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="66"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="73" t="s">
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="L51" s="74"/>
-      <c r="M51" s="74"/>
-      <c r="N51" s="74"/>
-      <c r="O51" s="74"/>
-      <c r="P51" s="74"/>
-      <c r="Q51" s="74"/>
-      <c r="R51" s="74"/>
-      <c r="S51" s="74"/>
-      <c r="T51" s="74"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="75"/>
+      <c r="L51" s="93"/>
+      <c r="M51" s="93"/>
+      <c r="N51" s="93"/>
+      <c r="O51" s="93"/>
+      <c r="P51" s="93"/>
+      <c r="Q51" s="93"/>
+      <c r="R51" s="93"/>
+      <c r="S51" s="93"/>
+      <c r="T51" s="93"/>
+      <c r="U51" s="93"/>
+      <c r="V51" s="94"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="68" t="s">
+      <c r="C52" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="69"/>
+      <c r="D52" s="60"/>
       <c r="E52" s="20" t="s">
         <v>23</v>
       </c>
@@ -3846,31 +3846,31 @@
       <c r="G52" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="70" t="s">
+      <c r="H52" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I52" s="70"/>
+      <c r="I52" s="61"/>
       <c r="J52" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K52" s="79" t="s">
+      <c r="K52" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
-      <c r="N52" s="80"/>
-      <c r="O52" s="81" t="s">
+      <c r="L52" s="88"/>
+      <c r="M52" s="88"/>
+      <c r="N52" s="88"/>
+      <c r="O52" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="P52" s="81"/>
-      <c r="Q52" s="81"/>
-      <c r="R52" s="81"/>
-      <c r="S52" s="82" t="s">
+      <c r="P52" s="89"/>
+      <c r="Q52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="T52" s="82"/>
-      <c r="U52" s="82"/>
-      <c r="V52" s="83"/>
+      <c r="T52" s="90"/>
+      <c r="U52" s="90"/>
+      <c r="V52" s="91"/>
     </row>
     <row r="53" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="12" t="s">
@@ -3939,129 +3939,129 @@
     </row>
     <row r="54" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B55" s="53" t="s">
+      <c r="B55" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="54"/>
-      <c r="D55" s="55" t="s">
+      <c r="C55" s="81"/>
+      <c r="D55" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="55"/>
-      <c r="H55" s="55"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="55"/>
-      <c r="K55" s="55"/>
-      <c r="L55" s="55"/>
-      <c r="M55" s="55"/>
-      <c r="N55" s="55"/>
-      <c r="O55" s="55"/>
-      <c r="P55" s="55"/>
-      <c r="Q55" s="55"/>
-      <c r="R55" s="55"/>
-      <c r="S55" s="56"/>
+      <c r="E55" s="82"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="82"/>
+      <c r="H55" s="82"/>
+      <c r="I55" s="82"/>
+      <c r="J55" s="82"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="82"/>
+      <c r="N55" s="82"/>
+      <c r="O55" s="82"/>
+      <c r="P55" s="82"/>
+      <c r="Q55" s="82"/>
+      <c r="R55" s="82"/>
+      <c r="S55" s="83"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B56" s="57" t="s">
+      <c r="B56" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="59" t="s">
+      <c r="C56" s="73"/>
+      <c r="D56" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="E56" s="59"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="59"/>
-      <c r="H56" s="59"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="59"/>
-      <c r="K56" s="59"/>
-      <c r="L56" s="59"/>
-      <c r="M56" s="59"/>
-      <c r="N56" s="59"/>
-      <c r="O56" s="59"/>
-      <c r="P56" s="59"/>
-      <c r="Q56" s="59"/>
-      <c r="R56" s="59"/>
-      <c r="S56" s="60"/>
+      <c r="E56" s="98"/>
+      <c r="F56" s="98"/>
+      <c r="G56" s="98"/>
+      <c r="H56" s="98"/>
+      <c r="I56" s="98"/>
+      <c r="J56" s="98"/>
+      <c r="K56" s="98"/>
+      <c r="L56" s="98"/>
+      <c r="M56" s="98"/>
+      <c r="N56" s="98"/>
+      <c r="O56" s="98"/>
+      <c r="P56" s="98"/>
+      <c r="Q56" s="98"/>
+      <c r="R56" s="98"/>
+      <c r="S56" s="99"/>
     </row>
     <row r="57" spans="1:25" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="61" t="s">
+      <c r="B57" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="62"/>
-      <c r="D57" s="63" t="s">
+      <c r="C57" s="63"/>
+      <c r="D57" s="100" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
-      <c r="I57" s="63"/>
-      <c r="J57" s="63"/>
-      <c r="K57" s="63"/>
-      <c r="L57" s="63"/>
-      <c r="M57" s="63"/>
-      <c r="N57" s="63"/>
-      <c r="O57" s="63"/>
-      <c r="P57" s="63"/>
-      <c r="Q57" s="63"/>
-      <c r="R57" s="63"/>
-      <c r="S57" s="64"/>
+      <c r="E57" s="100"/>
+      <c r="F57" s="100"/>
+      <c r="G57" s="100"/>
+      <c r="H57" s="100"/>
+      <c r="I57" s="100"/>
+      <c r="J57" s="100"/>
+      <c r="K57" s="100"/>
+      <c r="L57" s="100"/>
+      <c r="M57" s="100"/>
+      <c r="N57" s="100"/>
+      <c r="O57" s="100"/>
+      <c r="P57" s="100"/>
+      <c r="Q57" s="100"/>
+      <c r="R57" s="100"/>
+      <c r="S57" s="101"/>
     </row>
     <row r="59" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A59" s="31"/>
-      <c r="B59" s="71" t="s">
+      <c r="B59" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="71"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
-      <c r="F59" s="71"/>
-      <c r="G59" s="71"/>
-      <c r="H59" s="71"/>
-      <c r="I59" s="71"/>
-      <c r="J59" s="71"/>
-      <c r="K59" s="71"/>
-      <c r="L59" s="71"/>
-      <c r="M59" s="71"/>
-      <c r="N59" s="71"/>
-      <c r="O59" s="71"/>
-      <c r="P59" s="71"/>
-      <c r="Q59" s="71"/>
-      <c r="R59" s="71"/>
-      <c r="S59" s="71"/>
-      <c r="T59" s="71"/>
-      <c r="U59" s="71"/>
-      <c r="V59" s="71"/>
-      <c r="W59" s="71"/>
-      <c r="X59" s="71"/>
-      <c r="Y59" s="71"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="53"/>
+      <c r="L59" s="53"/>
+      <c r="M59" s="53"/>
+      <c r="N59" s="53"/>
+      <c r="O59" s="53"/>
+      <c r="P59" s="53"/>
+      <c r="Q59" s="53"/>
+      <c r="R59" s="53"/>
+      <c r="S59" s="53"/>
+      <c r="T59" s="53"/>
+      <c r="U59" s="53"/>
+      <c r="V59" s="53"/>
+      <c r="W59" s="53"/>
+      <c r="X59" s="53"/>
+      <c r="Y59" s="53"/>
     </row>
     <row r="61" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="65" t="s">
+      <c r="B61" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C61" s="65"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="65"/>
-      <c r="H61" s="65"/>
-      <c r="I61" s="65"/>
-      <c r="J61" s="65"/>
-      <c r="L61" s="72" t="s">
+      <c r="C61" s="85"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="85"/>
+      <c r="H61" s="85"/>
+      <c r="I61" s="85"/>
+      <c r="J61" s="85"/>
+      <c r="L61" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="M61" s="72"/>
-      <c r="N61" s="72"/>
-      <c r="O61" s="72"/>
-      <c r="P61" s="72"/>
-      <c r="Q61" s="72"/>
-      <c r="R61" s="72"/>
-      <c r="S61" s="72"/>
-      <c r="T61" s="72"/>
+      <c r="M61" s="86"/>
+      <c r="N61" s="86"/>
+      <c r="O61" s="86"/>
+      <c r="P61" s="86"/>
+      <c r="Q61" s="86"/>
+      <c r="R61" s="86"/>
+      <c r="S61" s="86"/>
+      <c r="T61" s="86"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
@@ -4121,36 +4121,36 @@
     </row>
     <row r="63" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="15"/>
-      <c r="C63" s="66" t="s">
+      <c r="C63" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="66"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="66"/>
-      <c r="H63" s="66"/>
-      <c r="I63" s="66"/>
-      <c r="J63" s="67"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="58"/>
       <c r="L63" s="15"/>
-      <c r="M63" s="66" t="s">
+      <c r="M63" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="N63" s="66"/>
-      <c r="O63" s="66"/>
-      <c r="P63" s="66"/>
-      <c r="Q63" s="66"/>
-      <c r="R63" s="66"/>
-      <c r="S63" s="66"/>
-      <c r="T63" s="67"/>
+      <c r="N63" s="57"/>
+      <c r="O63" s="57"/>
+      <c r="P63" s="57"/>
+      <c r="Q63" s="57"/>
+      <c r="R63" s="57"/>
+      <c r="S63" s="57"/>
+      <c r="T63" s="58"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="68" t="s">
+      <c r="C64" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="69"/>
+      <c r="D64" s="60"/>
       <c r="E64" s="20" t="s">
         <v>23</v>
       </c>
@@ -4160,20 +4160,20 @@
       <c r="G64" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H64" s="70" t="s">
+      <c r="H64" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I64" s="70"/>
+      <c r="I64" s="61"/>
       <c r="J64" s="21" t="s">
         <v>34</v>
       </c>
       <c r="L64" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M64" s="68" t="s">
+      <c r="M64" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="N64" s="69"/>
+      <c r="N64" s="60"/>
       <c r="O64" s="20" t="s">
         <v>23</v>
       </c>
@@ -4183,10 +4183,10 @@
       <c r="Q64" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="R64" s="70" t="s">
+      <c r="R64" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="S64" s="70"/>
+      <c r="S64" s="61"/>
       <c r="T64" s="21" t="s">
         <v>34</v>
       </c>
@@ -4249,105 +4249,105 @@
     </row>
     <row r="66" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B67" s="53" t="s">
+      <c r="B67" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C67" s="54"/>
-      <c r="D67" s="55" t="s">
+      <c r="C67" s="81"/>
+      <c r="D67" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="55"/>
-      <c r="K67" s="55"/>
-      <c r="L67" s="55"/>
-      <c r="M67" s="55"/>
-      <c r="N67" s="55"/>
-      <c r="O67" s="55"/>
-      <c r="P67" s="55"/>
-      <c r="Q67" s="55"/>
-      <c r="R67" s="55"/>
-      <c r="S67" s="56"/>
+      <c r="E67" s="82"/>
+      <c r="F67" s="82"/>
+      <c r="G67" s="82"/>
+      <c r="H67" s="82"/>
+      <c r="I67" s="82"/>
+      <c r="J67" s="82"/>
+      <c r="K67" s="82"/>
+      <c r="L67" s="82"/>
+      <c r="M67" s="82"/>
+      <c r="N67" s="82"/>
+      <c r="O67" s="82"/>
+      <c r="P67" s="82"/>
+      <c r="Q67" s="82"/>
+      <c r="R67" s="82"/>
+      <c r="S67" s="83"/>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B68" s="57" t="s">
+      <c r="B68" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="58"/>
-      <c r="D68" s="59" t="s">
+      <c r="C68" s="73"/>
+      <c r="D68" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="E68" s="59"/>
-      <c r="F68" s="59"/>
-      <c r="G68" s="59"/>
-      <c r="H68" s="59"/>
-      <c r="I68" s="59"/>
-      <c r="J68" s="59"/>
-      <c r="K68" s="59"/>
-      <c r="L68" s="59"/>
-      <c r="M68" s="59"/>
-      <c r="N68" s="59"/>
-      <c r="O68" s="59"/>
-      <c r="P68" s="59"/>
-      <c r="Q68" s="59"/>
-      <c r="R68" s="59"/>
-      <c r="S68" s="60"/>
+      <c r="E68" s="98"/>
+      <c r="F68" s="98"/>
+      <c r="G68" s="98"/>
+      <c r="H68" s="98"/>
+      <c r="I68" s="98"/>
+      <c r="J68" s="98"/>
+      <c r="K68" s="98"/>
+      <c r="L68" s="98"/>
+      <c r="M68" s="98"/>
+      <c r="N68" s="98"/>
+      <c r="O68" s="98"/>
+      <c r="P68" s="98"/>
+      <c r="Q68" s="98"/>
+      <c r="R68" s="98"/>
+      <c r="S68" s="99"/>
     </row>
     <row r="69" spans="1:25" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="61" t="s">
+      <c r="B69" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="63" t="s">
+      <c r="C69" s="63"/>
+      <c r="D69" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="E69" s="63"/>
-      <c r="F69" s="63"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="63"/>
-      <c r="I69" s="63"/>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="63"/>
-      <c r="M69" s="63"/>
-      <c r="N69" s="63"/>
-      <c r="O69" s="63"/>
-      <c r="P69" s="63"/>
-      <c r="Q69" s="63"/>
-      <c r="R69" s="63"/>
-      <c r="S69" s="64"/>
+      <c r="E69" s="100"/>
+      <c r="F69" s="100"/>
+      <c r="G69" s="100"/>
+      <c r="H69" s="100"/>
+      <c r="I69" s="100"/>
+      <c r="J69" s="100"/>
+      <c r="K69" s="100"/>
+      <c r="L69" s="100"/>
+      <c r="M69" s="100"/>
+      <c r="N69" s="100"/>
+      <c r="O69" s="100"/>
+      <c r="P69" s="100"/>
+      <c r="Q69" s="100"/>
+      <c r="R69" s="100"/>
+      <c r="S69" s="101"/>
     </row>
     <row r="71" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A71" s="31"/>
-      <c r="B71" s="71" t="s">
+      <c r="B71" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C71" s="71"/>
-      <c r="D71" s="71"/>
-      <c r="E71" s="71"/>
-      <c r="F71" s="71"/>
-      <c r="G71" s="71"/>
-      <c r="H71" s="71"/>
-      <c r="I71" s="71"/>
-      <c r="J71" s="71"/>
-      <c r="K71" s="71"/>
-      <c r="L71" s="71"/>
-      <c r="M71" s="71"/>
-      <c r="N71" s="71"/>
-      <c r="O71" s="71"/>
-      <c r="P71" s="71"/>
-      <c r="Q71" s="71"/>
-      <c r="R71" s="71"/>
-      <c r="S71" s="71"/>
-      <c r="T71" s="71"/>
-      <c r="U71" s="71"/>
-      <c r="V71" s="71"/>
-      <c r="W71" s="71"/>
-      <c r="X71" s="71"/>
-      <c r="Y71" s="71"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
+      <c r="L71" s="53"/>
+      <c r="M71" s="53"/>
+      <c r="N71" s="53"/>
+      <c r="O71" s="53"/>
+      <c r="P71" s="53"/>
+      <c r="Q71" s="53"/>
+      <c r="R71" s="53"/>
+      <c r="S71" s="53"/>
+      <c r="T71" s="53"/>
+      <c r="U71" s="53"/>
+      <c r="V71" s="53"/>
+      <c r="W71" s="53"/>
+      <c r="X71" s="53"/>
+      <c r="Y71" s="53"/>
     </row>
     <row r="72" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
@@ -4393,31 +4393,31 @@
     </row>
     <row r="74" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="15"/>
-      <c r="C74" s="66" t="s">
+      <c r="C74" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="66"/>
-      <c r="E74" s="66"/>
-      <c r="F74" s="66"/>
-      <c r="G74" s="66"/>
-      <c r="H74" s="66"/>
-      <c r="I74" s="66"/>
-      <c r="J74" s="67"/>
-      <c r="K74" s="73" t="s">
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="57"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="58"/>
+      <c r="K74" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="L74" s="74"/>
-      <c r="M74" s="74"/>
-      <c r="N74" s="75"/>
+      <c r="L74" s="93"/>
+      <c r="M74" s="93"/>
+      <c r="N74" s="94"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B75" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C75" s="68" t="s">
+      <c r="C75" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="69"/>
+      <c r="D75" s="60"/>
       <c r="E75" s="20" t="s">
         <v>23</v>
       </c>
@@ -4427,19 +4427,19 @@
       <c r="G75" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H75" s="70" t="s">
+      <c r="H75" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I75" s="70"/>
+      <c r="I75" s="61"/>
       <c r="J75" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K75" s="76" t="s">
+      <c r="K75" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="L75" s="77"/>
-      <c r="M75" s="77"/>
-      <c r="N75" s="78"/>
+      <c r="L75" s="96"/>
+      <c r="M75" s="96"/>
+      <c r="N75" s="97"/>
     </row>
     <row r="76" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="12" t="s">
@@ -4484,129 +4484,129 @@
     </row>
     <row r="77" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B78" s="53" t="s">
+      <c r="B78" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C78" s="54"/>
-      <c r="D78" s="55" t="s">
+      <c r="C78" s="81"/>
+      <c r="D78" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E78" s="55"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="55"/>
-      <c r="H78" s="55"/>
-      <c r="I78" s="55"/>
-      <c r="J78" s="55"/>
-      <c r="K78" s="55"/>
-      <c r="L78" s="55"/>
-      <c r="M78" s="55"/>
-      <c r="N78" s="55"/>
-      <c r="O78" s="55"/>
-      <c r="P78" s="55"/>
-      <c r="Q78" s="55"/>
-      <c r="R78" s="55"/>
-      <c r="S78" s="56"/>
+      <c r="E78" s="82"/>
+      <c r="F78" s="82"/>
+      <c r="G78" s="82"/>
+      <c r="H78" s="82"/>
+      <c r="I78" s="82"/>
+      <c r="J78" s="82"/>
+      <c r="K78" s="82"/>
+      <c r="L78" s="82"/>
+      <c r="M78" s="82"/>
+      <c r="N78" s="82"/>
+      <c r="O78" s="82"/>
+      <c r="P78" s="82"/>
+      <c r="Q78" s="82"/>
+      <c r="R78" s="82"/>
+      <c r="S78" s="83"/>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B79" s="57" t="s">
+      <c r="B79" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C79" s="58"/>
-      <c r="D79" s="59" t="s">
+      <c r="C79" s="73"/>
+      <c r="D79" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="E79" s="59"/>
-      <c r="F79" s="59"/>
-      <c r="G79" s="59"/>
-      <c r="H79" s="59"/>
-      <c r="I79" s="59"/>
-      <c r="J79" s="59"/>
-      <c r="K79" s="59"/>
-      <c r="L79" s="59"/>
-      <c r="M79" s="59"/>
-      <c r="N79" s="59"/>
-      <c r="O79" s="59"/>
-      <c r="P79" s="59"/>
-      <c r="Q79" s="59"/>
-      <c r="R79" s="59"/>
-      <c r="S79" s="60"/>
+      <c r="E79" s="98"/>
+      <c r="F79" s="98"/>
+      <c r="G79" s="98"/>
+      <c r="H79" s="98"/>
+      <c r="I79" s="98"/>
+      <c r="J79" s="98"/>
+      <c r="K79" s="98"/>
+      <c r="L79" s="98"/>
+      <c r="M79" s="98"/>
+      <c r="N79" s="98"/>
+      <c r="O79" s="98"/>
+      <c r="P79" s="98"/>
+      <c r="Q79" s="98"/>
+      <c r="R79" s="98"/>
+      <c r="S79" s="99"/>
     </row>
     <row r="80" spans="1:25" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="61" t="s">
+      <c r="B80" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="62"/>
-      <c r="D80" s="63" t="s">
+      <c r="C80" s="63"/>
+      <c r="D80" s="100" t="s">
         <v>104</v>
       </c>
-      <c r="E80" s="63"/>
-      <c r="F80" s="63"/>
-      <c r="G80" s="63"/>
-      <c r="H80" s="63"/>
-      <c r="I80" s="63"/>
-      <c r="J80" s="63"/>
-      <c r="K80" s="63"/>
-      <c r="L80" s="63"/>
-      <c r="M80" s="63"/>
-      <c r="N80" s="63"/>
-      <c r="O80" s="63"/>
-      <c r="P80" s="63"/>
-      <c r="Q80" s="63"/>
-      <c r="R80" s="63"/>
-      <c r="S80" s="64"/>
+      <c r="E80" s="100"/>
+      <c r="F80" s="100"/>
+      <c r="G80" s="100"/>
+      <c r="H80" s="100"/>
+      <c r="I80" s="100"/>
+      <c r="J80" s="100"/>
+      <c r="K80" s="100"/>
+      <c r="L80" s="100"/>
+      <c r="M80" s="100"/>
+      <c r="N80" s="100"/>
+      <c r="O80" s="100"/>
+      <c r="P80" s="100"/>
+      <c r="Q80" s="100"/>
+      <c r="R80" s="100"/>
+      <c r="S80" s="101"/>
     </row>
     <row r="82" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A82" s="31"/>
-      <c r="B82" s="71" t="s">
+      <c r="B82" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C82" s="71"/>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
-      <c r="F82" s="71"/>
-      <c r="G82" s="71"/>
-      <c r="H82" s="71"/>
-      <c r="I82" s="71"/>
-      <c r="J82" s="71"/>
-      <c r="K82" s="71"/>
-      <c r="L82" s="71"/>
-      <c r="M82" s="71"/>
-      <c r="N82" s="71"/>
-      <c r="O82" s="71"/>
-      <c r="P82" s="71"/>
-      <c r="Q82" s="71"/>
-      <c r="R82" s="71"/>
-      <c r="S82" s="71"/>
-      <c r="T82" s="71"/>
-      <c r="U82" s="71"/>
-      <c r="V82" s="71"/>
-      <c r="W82" s="71"/>
-      <c r="X82" s="71"/>
-      <c r="Y82" s="71"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
+      <c r="E82" s="53"/>
+      <c r="F82" s="53"/>
+      <c r="G82" s="53"/>
+      <c r="H82" s="53"/>
+      <c r="I82" s="53"/>
+      <c r="J82" s="53"/>
+      <c r="K82" s="53"/>
+      <c r="L82" s="53"/>
+      <c r="M82" s="53"/>
+      <c r="N82" s="53"/>
+      <c r="O82" s="53"/>
+      <c r="P82" s="53"/>
+      <c r="Q82" s="53"/>
+      <c r="R82" s="53"/>
+      <c r="S82" s="53"/>
+      <c r="T82" s="53"/>
+      <c r="U82" s="53"/>
+      <c r="V82" s="53"/>
+      <c r="W82" s="53"/>
+      <c r="X82" s="53"/>
+      <c r="Y82" s="53"/>
     </row>
     <row r="84" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="65" t="s">
+      <c r="B84" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C84" s="65"/>
-      <c r="D84" s="65"/>
-      <c r="E84" s="65"/>
-      <c r="F84" s="65"/>
-      <c r="G84" s="65"/>
-      <c r="H84" s="65"/>
-      <c r="I84" s="65"/>
-      <c r="J84" s="65"/>
-      <c r="L84" s="72" t="s">
+      <c r="C84" s="85"/>
+      <c r="D84" s="85"/>
+      <c r="E84" s="85"/>
+      <c r="F84" s="85"/>
+      <c r="G84" s="85"/>
+      <c r="H84" s="85"/>
+      <c r="I84" s="85"/>
+      <c r="J84" s="85"/>
+      <c r="L84" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="M84" s="72"/>
-      <c r="N84" s="72"/>
-      <c r="O84" s="72"/>
-      <c r="P84" s="72"/>
-      <c r="Q84" s="72"/>
-      <c r="R84" s="72"/>
-      <c r="S84" s="72"/>
-      <c r="T84" s="72"/>
+      <c r="M84" s="86"/>
+      <c r="N84" s="86"/>
+      <c r="O84" s="86"/>
+      <c r="P84" s="86"/>
+      <c r="Q84" s="86"/>
+      <c r="R84" s="86"/>
+      <c r="S84" s="86"/>
+      <c r="T84" s="86"/>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B85" s="9" t="s">
@@ -4666,36 +4666,36 @@
     </row>
     <row r="86" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="15"/>
-      <c r="C86" s="66" t="s">
+      <c r="C86" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D86" s="66"/>
-      <c r="E86" s="66"/>
-      <c r="F86" s="66"/>
-      <c r="G86" s="66"/>
-      <c r="H86" s="66"/>
-      <c r="I86" s="66"/>
-      <c r="J86" s="67"/>
+      <c r="D86" s="57"/>
+      <c r="E86" s="57"/>
+      <c r="F86" s="57"/>
+      <c r="G86" s="57"/>
+      <c r="H86" s="57"/>
+      <c r="I86" s="57"/>
+      <c r="J86" s="58"/>
       <c r="L86" s="15"/>
-      <c r="M86" s="66" t="s">
+      <c r="M86" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="N86" s="66"/>
-      <c r="O86" s="66"/>
-      <c r="P86" s="66"/>
-      <c r="Q86" s="66"/>
-      <c r="R86" s="66"/>
-      <c r="S86" s="66"/>
-      <c r="T86" s="67"/>
+      <c r="N86" s="57"/>
+      <c r="O86" s="57"/>
+      <c r="P86" s="57"/>
+      <c r="Q86" s="57"/>
+      <c r="R86" s="57"/>
+      <c r="S86" s="57"/>
+      <c r="T86" s="58"/>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B87" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="69"/>
+      <c r="D87" s="60"/>
       <c r="E87" s="20" t="s">
         <v>23</v>
       </c>
@@ -4705,20 +4705,20 @@
       <c r="G87" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H87" s="70" t="s">
+      <c r="H87" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I87" s="70"/>
+      <c r="I87" s="61"/>
       <c r="J87" s="21" t="s">
         <v>34</v>
       </c>
       <c r="L87" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M87" s="68" t="s">
+      <c r="M87" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="N87" s="69"/>
+      <c r="N87" s="60"/>
       <c r="O87" s="20" t="s">
         <v>23</v>
       </c>
@@ -4728,10 +4728,10 @@
       <c r="Q87" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="R87" s="70" t="s">
+      <c r="R87" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="S87" s="70"/>
+      <c r="S87" s="61"/>
       <c r="T87" s="21" t="s">
         <v>34</v>
       </c>
@@ -4794,105 +4794,105 @@
     </row>
     <row r="89" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B90" s="53" t="s">
+      <c r="B90" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C90" s="54"/>
-      <c r="D90" s="55" t="s">
+      <c r="C90" s="81"/>
+      <c r="D90" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E90" s="55"/>
-      <c r="F90" s="55"/>
-      <c r="G90" s="55"/>
-      <c r="H90" s="55"/>
-      <c r="I90" s="55"/>
-      <c r="J90" s="55"/>
-      <c r="K90" s="55"/>
-      <c r="L90" s="55"/>
-      <c r="M90" s="55"/>
-      <c r="N90" s="55"/>
-      <c r="O90" s="55"/>
-      <c r="P90" s="55"/>
-      <c r="Q90" s="55"/>
-      <c r="R90" s="55"/>
-      <c r="S90" s="56"/>
+      <c r="E90" s="82"/>
+      <c r="F90" s="82"/>
+      <c r="G90" s="82"/>
+      <c r="H90" s="82"/>
+      <c r="I90" s="82"/>
+      <c r="J90" s="82"/>
+      <c r="K90" s="82"/>
+      <c r="L90" s="82"/>
+      <c r="M90" s="82"/>
+      <c r="N90" s="82"/>
+      <c r="O90" s="82"/>
+      <c r="P90" s="82"/>
+      <c r="Q90" s="82"/>
+      <c r="R90" s="82"/>
+      <c r="S90" s="83"/>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B91" s="57" t="s">
+      <c r="B91" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C91" s="58"/>
-      <c r="D91" s="59" t="s">
+      <c r="C91" s="73"/>
+      <c r="D91" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="E91" s="59"/>
-      <c r="F91" s="59"/>
-      <c r="G91" s="59"/>
-      <c r="H91" s="59"/>
-      <c r="I91" s="59"/>
-      <c r="J91" s="59"/>
-      <c r="K91" s="59"/>
-      <c r="L91" s="59"/>
-      <c r="M91" s="59"/>
-      <c r="N91" s="59"/>
-      <c r="O91" s="59"/>
-      <c r="P91" s="59"/>
-      <c r="Q91" s="59"/>
-      <c r="R91" s="59"/>
-      <c r="S91" s="60"/>
+      <c r="E91" s="98"/>
+      <c r="F91" s="98"/>
+      <c r="G91" s="98"/>
+      <c r="H91" s="98"/>
+      <c r="I91" s="98"/>
+      <c r="J91" s="98"/>
+      <c r="K91" s="98"/>
+      <c r="L91" s="98"/>
+      <c r="M91" s="98"/>
+      <c r="N91" s="98"/>
+      <c r="O91" s="98"/>
+      <c r="P91" s="98"/>
+      <c r="Q91" s="98"/>
+      <c r="R91" s="98"/>
+      <c r="S91" s="99"/>
     </row>
     <row r="92" spans="1:25" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="61" t="s">
+      <c r="B92" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C92" s="62"/>
-      <c r="D92" s="63" t="s">
+      <c r="C92" s="63"/>
+      <c r="D92" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="E92" s="63"/>
-      <c r="F92" s="63"/>
-      <c r="G92" s="63"/>
-      <c r="H92" s="63"/>
-      <c r="I92" s="63"/>
-      <c r="J92" s="63"/>
-      <c r="K92" s="63"/>
-      <c r="L92" s="63"/>
-      <c r="M92" s="63"/>
-      <c r="N92" s="63"/>
-      <c r="O92" s="63"/>
-      <c r="P92" s="63"/>
-      <c r="Q92" s="63"/>
-      <c r="R92" s="63"/>
-      <c r="S92" s="64"/>
+      <c r="E92" s="100"/>
+      <c r="F92" s="100"/>
+      <c r="G92" s="100"/>
+      <c r="H92" s="100"/>
+      <c r="I92" s="100"/>
+      <c r="J92" s="100"/>
+      <c r="K92" s="100"/>
+      <c r="L92" s="100"/>
+      <c r="M92" s="100"/>
+      <c r="N92" s="100"/>
+      <c r="O92" s="100"/>
+      <c r="P92" s="100"/>
+      <c r="Q92" s="100"/>
+      <c r="R92" s="100"/>
+      <c r="S92" s="101"/>
     </row>
     <row r="94" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A94" s="31"/>
-      <c r="B94" s="71" t="s">
+      <c r="B94" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="71"/>
-      <c r="D94" s="71"/>
-      <c r="E94" s="71"/>
-      <c r="F94" s="71"/>
-      <c r="G94" s="71"/>
-      <c r="H94" s="71"/>
-      <c r="I94" s="71"/>
-      <c r="J94" s="71"/>
-      <c r="K94" s="71"/>
-      <c r="L94" s="71"/>
-      <c r="M94" s="71"/>
-      <c r="N94" s="71"/>
-      <c r="O94" s="71"/>
-      <c r="P94" s="71"/>
-      <c r="Q94" s="71"/>
-      <c r="R94" s="71"/>
-      <c r="S94" s="71"/>
-      <c r="T94" s="71"/>
-      <c r="U94" s="71"/>
-      <c r="V94" s="71"/>
-      <c r="W94" s="71"/>
-      <c r="X94" s="71"/>
-      <c r="Y94" s="71"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="53"/>
+      <c r="E94" s="53"/>
+      <c r="F94" s="53"/>
+      <c r="G94" s="53"/>
+      <c r="H94" s="53"/>
+      <c r="I94" s="53"/>
+      <c r="J94" s="53"/>
+      <c r="K94" s="53"/>
+      <c r="L94" s="53"/>
+      <c r="M94" s="53"/>
+      <c r="N94" s="53"/>
+      <c r="O94" s="53"/>
+      <c r="P94" s="53"/>
+      <c r="Q94" s="53"/>
+      <c r="R94" s="53"/>
+      <c r="S94" s="53"/>
+      <c r="T94" s="53"/>
+      <c r="U94" s="53"/>
+      <c r="V94" s="53"/>
+      <c r="W94" s="53"/>
+      <c r="X94" s="53"/>
+      <c r="Y94" s="53"/>
     </row>
     <row r="95" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
@@ -4926,25 +4926,25 @@
     </row>
     <row r="97" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B97" s="15"/>
-      <c r="C97" s="66" t="s">
+      <c r="C97" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D97" s="66"/>
-      <c r="E97" s="66"/>
-      <c r="F97" s="66"/>
-      <c r="G97" s="66"/>
-      <c r="H97" s="66"/>
-      <c r="I97" s="66"/>
-      <c r="J97" s="67"/>
+      <c r="D97" s="57"/>
+      <c r="E97" s="57"/>
+      <c r="F97" s="57"/>
+      <c r="G97" s="57"/>
+      <c r="H97" s="57"/>
+      <c r="I97" s="57"/>
+      <c r="J97" s="58"/>
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B98" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C98" s="68" t="s">
+      <c r="C98" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D98" s="69"/>
+      <c r="D98" s="60"/>
       <c r="E98" s="20" t="s">
         <v>23</v>
       </c>
@@ -4954,10 +4954,10 @@
       <c r="G98" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H98" s="70" t="s">
+      <c r="H98" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I98" s="70"/>
+      <c r="I98" s="61"/>
       <c r="J98" s="21" t="s">
         <v>34</v>
       </c>
@@ -4993,118 +4993,118 @@
     </row>
     <row r="100" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="101" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B101" s="53" t="s">
+      <c r="B101" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C101" s="54"/>
-      <c r="D101" s="55" t="s">
+      <c r="C101" s="81"/>
+      <c r="D101" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E101" s="55"/>
-      <c r="F101" s="55"/>
-      <c r="G101" s="55"/>
-      <c r="H101" s="55"/>
-      <c r="I101" s="55"/>
-      <c r="J101" s="55"/>
-      <c r="K101" s="55"/>
-      <c r="L101" s="55"/>
-      <c r="M101" s="55"/>
-      <c r="N101" s="55"/>
-      <c r="O101" s="55"/>
-      <c r="P101" s="55"/>
-      <c r="Q101" s="55"/>
-      <c r="R101" s="55"/>
-      <c r="S101" s="56"/>
+      <c r="E101" s="82"/>
+      <c r="F101" s="82"/>
+      <c r="G101" s="82"/>
+      <c r="H101" s="82"/>
+      <c r="I101" s="82"/>
+      <c r="J101" s="82"/>
+      <c r="K101" s="82"/>
+      <c r="L101" s="82"/>
+      <c r="M101" s="82"/>
+      <c r="N101" s="82"/>
+      <c r="O101" s="82"/>
+      <c r="P101" s="82"/>
+      <c r="Q101" s="82"/>
+      <c r="R101" s="82"/>
+      <c r="S101" s="83"/>
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B102" s="57" t="s">
+      <c r="B102" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C102" s="58"/>
-      <c r="D102" s="59" t="s">
+      <c r="C102" s="73"/>
+      <c r="D102" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="E102" s="59"/>
-      <c r="F102" s="59"/>
-      <c r="G102" s="59"/>
-      <c r="H102" s="59"/>
-      <c r="I102" s="59"/>
-      <c r="J102" s="59"/>
-      <c r="K102" s="59"/>
-      <c r="L102" s="59"/>
-      <c r="M102" s="59"/>
-      <c r="N102" s="59"/>
-      <c r="O102" s="59"/>
-      <c r="P102" s="59"/>
-      <c r="Q102" s="59"/>
-      <c r="R102" s="59"/>
-      <c r="S102" s="60"/>
+      <c r="E102" s="98"/>
+      <c r="F102" s="98"/>
+      <c r="G102" s="98"/>
+      <c r="H102" s="98"/>
+      <c r="I102" s="98"/>
+      <c r="J102" s="98"/>
+      <c r="K102" s="98"/>
+      <c r="L102" s="98"/>
+      <c r="M102" s="98"/>
+      <c r="N102" s="98"/>
+      <c r="O102" s="98"/>
+      <c r="P102" s="98"/>
+      <c r="Q102" s="98"/>
+      <c r="R102" s="98"/>
+      <c r="S102" s="99"/>
     </row>
     <row r="103" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="61" t="s">
+      <c r="B103" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C103" s="62"/>
-      <c r="D103" s="63" t="s">
+      <c r="C103" s="63"/>
+      <c r="D103" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="E103" s="63"/>
-      <c r="F103" s="63"/>
-      <c r="G103" s="63"/>
-      <c r="H103" s="63"/>
-      <c r="I103" s="63"/>
-      <c r="J103" s="63"/>
-      <c r="K103" s="63"/>
-      <c r="L103" s="63"/>
-      <c r="M103" s="63"/>
-      <c r="N103" s="63"/>
-      <c r="O103" s="63"/>
-      <c r="P103" s="63"/>
-      <c r="Q103" s="63"/>
-      <c r="R103" s="63"/>
-      <c r="S103" s="64"/>
+      <c r="E103" s="100"/>
+      <c r="F103" s="100"/>
+      <c r="G103" s="100"/>
+      <c r="H103" s="100"/>
+      <c r="I103" s="100"/>
+      <c r="J103" s="100"/>
+      <c r="K103" s="100"/>
+      <c r="L103" s="100"/>
+      <c r="M103" s="100"/>
+      <c r="N103" s="100"/>
+      <c r="O103" s="100"/>
+      <c r="P103" s="100"/>
+      <c r="Q103" s="100"/>
+      <c r="R103" s="100"/>
+      <c r="S103" s="101"/>
     </row>
     <row r="105" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A105" s="31"/>
-      <c r="B105" s="71" t="s">
+      <c r="B105" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C105" s="71"/>
-      <c r="D105" s="71"/>
-      <c r="E105" s="71"/>
-      <c r="F105" s="71"/>
-      <c r="G105" s="71"/>
-      <c r="H105" s="71"/>
-      <c r="I105" s="71"/>
-      <c r="J105" s="71"/>
-      <c r="K105" s="71"/>
-      <c r="L105" s="71"/>
-      <c r="M105" s="71"/>
-      <c r="N105" s="71"/>
-      <c r="O105" s="71"/>
-      <c r="P105" s="71"/>
-      <c r="Q105" s="71"/>
-      <c r="R105" s="71"/>
-      <c r="S105" s="71"/>
-      <c r="T105" s="71"/>
-      <c r="U105" s="71"/>
-      <c r="V105" s="71"/>
-      <c r="W105" s="71"/>
-      <c r="X105" s="71"/>
-      <c r="Y105" s="71"/>
+      <c r="C105" s="53"/>
+      <c r="D105" s="53"/>
+      <c r="E105" s="53"/>
+      <c r="F105" s="53"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="53"/>
+      <c r="I105" s="53"/>
+      <c r="J105" s="53"/>
+      <c r="K105" s="53"/>
+      <c r="L105" s="53"/>
+      <c r="M105" s="53"/>
+      <c r="N105" s="53"/>
+      <c r="O105" s="53"/>
+      <c r="P105" s="53"/>
+      <c r="Q105" s="53"/>
+      <c r="R105" s="53"/>
+      <c r="S105" s="53"/>
+      <c r="T105" s="53"/>
+      <c r="U105" s="53"/>
+      <c r="V105" s="53"/>
+      <c r="W105" s="53"/>
+      <c r="X105" s="53"/>
+      <c r="Y105" s="53"/>
     </row>
     <row r="107" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="65" t="s">
+      <c r="B107" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C107" s="65"/>
-      <c r="D107" s="65"/>
-      <c r="E107" s="65"/>
-      <c r="F107" s="65"/>
-      <c r="G107" s="65"/>
-      <c r="H107" s="65"/>
-      <c r="I107" s="65"/>
-      <c r="J107" s="65"/>
+      <c r="C107" s="85"/>
+      <c r="D107" s="85"/>
+      <c r="E107" s="85"/>
+      <c r="F107" s="85"/>
+      <c r="G107" s="85"/>
+      <c r="H107" s="85"/>
+      <c r="I107" s="85"/>
+      <c r="J107" s="85"/>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B108" s="9" t="s">
@@ -5137,25 +5137,25 @@
     </row>
     <row r="109" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B109" s="15"/>
-      <c r="C109" s="66" t="s">
+      <c r="C109" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="D109" s="66"/>
-      <c r="E109" s="66"/>
-      <c r="F109" s="66"/>
-      <c r="G109" s="66"/>
-      <c r="H109" s="66"/>
-      <c r="I109" s="66"/>
-      <c r="J109" s="67"/>
+      <c r="D109" s="57"/>
+      <c r="E109" s="57"/>
+      <c r="F109" s="57"/>
+      <c r="G109" s="57"/>
+      <c r="H109" s="57"/>
+      <c r="I109" s="57"/>
+      <c r="J109" s="58"/>
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B110" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C110" s="68" t="s">
+      <c r="C110" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D110" s="69"/>
+      <c r="D110" s="60"/>
       <c r="E110" s="20" t="s">
         <v>23</v>
       </c>
@@ -5165,10 +5165,10 @@
       <c r="G110" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H110" s="70" t="s">
+      <c r="H110" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I110" s="70"/>
+      <c r="I110" s="61"/>
       <c r="J110" s="21" t="s">
         <v>34</v>
       </c>
@@ -5204,79 +5204,178 @@
     </row>
     <row r="112" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="113" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B113" s="53" t="s">
+      <c r="B113" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C113" s="54"/>
-      <c r="D113" s="55" t="s">
+      <c r="C113" s="81"/>
+      <c r="D113" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E113" s="55"/>
-      <c r="F113" s="55"/>
-      <c r="G113" s="55"/>
-      <c r="H113" s="55"/>
-      <c r="I113" s="55"/>
-      <c r="J113" s="55"/>
-      <c r="K113" s="55"/>
-      <c r="L113" s="55"/>
-      <c r="M113" s="55"/>
-      <c r="N113" s="55"/>
-      <c r="O113" s="55"/>
-      <c r="P113" s="55"/>
-      <c r="Q113" s="55"/>
-      <c r="R113" s="55"/>
-      <c r="S113" s="56"/>
+      <c r="E113" s="82"/>
+      <c r="F113" s="82"/>
+      <c r="G113" s="82"/>
+      <c r="H113" s="82"/>
+      <c r="I113" s="82"/>
+      <c r="J113" s="82"/>
+      <c r="K113" s="82"/>
+      <c r="L113" s="82"/>
+      <c r="M113" s="82"/>
+      <c r="N113" s="82"/>
+      <c r="O113" s="82"/>
+      <c r="P113" s="82"/>
+      <c r="Q113" s="82"/>
+      <c r="R113" s="82"/>
+      <c r="S113" s="83"/>
     </row>
     <row r="114" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B114" s="57" t="s">
+      <c r="B114" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="58"/>
-      <c r="D114" s="59" t="s">
+      <c r="C114" s="73"/>
+      <c r="D114" s="98" t="s">
         <v>105</v>
       </c>
-      <c r="E114" s="59"/>
-      <c r="F114" s="59"/>
-      <c r="G114" s="59"/>
-      <c r="H114" s="59"/>
-      <c r="I114" s="59"/>
-      <c r="J114" s="59"/>
-      <c r="K114" s="59"/>
-      <c r="L114" s="59"/>
-      <c r="M114" s="59"/>
-      <c r="N114" s="59"/>
-      <c r="O114" s="59"/>
-      <c r="P114" s="59"/>
-      <c r="Q114" s="59"/>
-      <c r="R114" s="59"/>
-      <c r="S114" s="60"/>
+      <c r="E114" s="98"/>
+      <c r="F114" s="98"/>
+      <c r="G114" s="98"/>
+      <c r="H114" s="98"/>
+      <c r="I114" s="98"/>
+      <c r="J114" s="98"/>
+      <c r="K114" s="98"/>
+      <c r="L114" s="98"/>
+      <c r="M114" s="98"/>
+      <c r="N114" s="98"/>
+      <c r="O114" s="98"/>
+      <c r="P114" s="98"/>
+      <c r="Q114" s="98"/>
+      <c r="R114" s="98"/>
+      <c r="S114" s="99"/>
     </row>
     <row r="115" spans="2:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="61" t="s">
+      <c r="B115" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C115" s="62"/>
-      <c r="D115" s="63" t="s">
+      <c r="C115" s="63"/>
+      <c r="D115" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="E115" s="63"/>
-      <c r="F115" s="63"/>
-      <c r="G115" s="63"/>
-      <c r="H115" s="63"/>
-      <c r="I115" s="63"/>
-      <c r="J115" s="63"/>
-      <c r="K115" s="63"/>
-      <c r="L115" s="63"/>
-      <c r="M115" s="63"/>
-      <c r="N115" s="63"/>
-      <c r="O115" s="63"/>
-      <c r="P115" s="63"/>
-      <c r="Q115" s="63"/>
-      <c r="R115" s="63"/>
-      <c r="S115" s="64"/>
+      <c r="E115" s="100"/>
+      <c r="F115" s="100"/>
+      <c r="G115" s="100"/>
+      <c r="H115" s="100"/>
+      <c r="I115" s="100"/>
+      <c r="J115" s="100"/>
+      <c r="K115" s="100"/>
+      <c r="L115" s="100"/>
+      <c r="M115" s="100"/>
+      <c r="N115" s="100"/>
+      <c r="O115" s="100"/>
+      <c r="P115" s="100"/>
+      <c r="Q115" s="100"/>
+      <c r="R115" s="100"/>
+      <c r="S115" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:S57"/>
+    <mergeCell ref="D101:S101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:S102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:S103"/>
+    <mergeCell ref="B82:Y82"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:S113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:S114"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:S67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:S68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:S69"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:S115"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:S90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="D91:S91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:S92"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:S78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D79:S79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:S80"/>
+    <mergeCell ref="B107:J107"/>
+    <mergeCell ref="C109:J109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="B94:Y94"/>
+    <mergeCell ref="C97:J97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="B105:Y105"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="D33:S33"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:S55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:S56"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="L37:T37"/>
+    <mergeCell ref="M39:T39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:S43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:S44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:S45"/>
+    <mergeCell ref="B84:J84"/>
+    <mergeCell ref="C86:J86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="L84:T84"/>
+    <mergeCell ref="M86:T86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="R87:S87"/>
+    <mergeCell ref="B71:Y71"/>
+    <mergeCell ref="C74:J74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="B61:J61"/>
+    <mergeCell ref="C63:J63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="L61:T61"/>
+    <mergeCell ref="M63:T63"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="B48:Y48"/>
+    <mergeCell ref="C51:J51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B59:Y59"/>
+    <mergeCell ref="K52:N52"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="S52:V52"/>
+    <mergeCell ref="K51:V51"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:S31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:S32"/>
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="B2:Y2"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:P5"/>
@@ -5301,105 +5400,6 @@
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:J14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="B61:J61"/>
-    <mergeCell ref="C63:J63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="L61:T61"/>
-    <mergeCell ref="M63:T63"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="B48:Y48"/>
-    <mergeCell ref="C51:J51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="B59:Y59"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="S52:V52"/>
-    <mergeCell ref="K51:V51"/>
-    <mergeCell ref="B84:J84"/>
-    <mergeCell ref="C86:J86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="L84:T84"/>
-    <mergeCell ref="M86:T86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="R87:S87"/>
-    <mergeCell ref="B71:Y71"/>
-    <mergeCell ref="C74:J74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:S31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:S32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:S33"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:S55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:S56"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="L37:T37"/>
-    <mergeCell ref="M39:T39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:S115"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:S90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="D91:S91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:S92"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:S78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="D79:S79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:S80"/>
-    <mergeCell ref="B107:J107"/>
-    <mergeCell ref="C109:J109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="B94:Y94"/>
-    <mergeCell ref="C97:J97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="B105:Y105"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:S43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:S44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:S45"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:S113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:S114"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:S67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:S68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:S69"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:S57"/>
-    <mergeCell ref="D101:S101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:S102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:S103"/>
-    <mergeCell ref="B82:Y82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- updated bootloader interface specification doc - added boot interface print version doc
</commit_message>
<xml_diff>
--- a/doc/Bootloader_Interface_Specifications.xlsx
+++ b/doc/Bootloader_Interface_Specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SELTRON\zigamiklosic\Personal\HomeWork\ECS_Bootloader\OrderBob\middleware\boot\boot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10132D7-CD53-4825-A2EC-8362BA333508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEB07DC-8406-4A9A-811F-E0876942AB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23535" yWindow="660" windowWidth="22620" windowHeight="14145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="142">
   <si>
     <t>Document status:</t>
   </si>
@@ -443,405 +443,6 @@
     <t>On Receive</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Command type
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Connect</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x11</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Connect response</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x20</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prepare</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x21</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prepare response</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x30</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Flash data</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x31</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Flash data response</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x41</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Exit (jump to application)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x41:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Exit response</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>other values</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Ignore</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>size[7:0]</t>
   </si>
   <si>
@@ -869,19 +470,10 @@
     <t>The Connect command is being generated by Bootloader Manager (PC application) when starting a bootloading procedure.</t>
   </si>
   <si>
-    <t>Connect Response command is being generated by Bootloader (embedded) on reception of Connect command.</t>
-  </si>
-  <si>
-    <t>Prepare response command is being generated by Bootloader (embedded) on reception of Prepare command.</t>
-  </si>
-  <si>
     <t>The Prepare command is being generated by Bootloader Manager (PC application) after successfull connection to bootloader.</t>
   </si>
   <si>
     <t>The Flash Data command is being generated by Bootloader Manager (PC application) after successfull preparation phase (flash erase).</t>
-  </si>
-  <si>
-    <t>Exit response command is being generated by Bootloader (embedded) on reception of Exit command.</t>
   </si>
   <si>
     <t xml:space="preserve"> - Little Endiannes 
@@ -1077,347 +669,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">New firmware image hardware support version. Version is coded as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">hexadecimal format </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xMMmmddtt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, where:  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - MM: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>major software number,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- - mm: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>minor software number,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- - dd: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>develop software number,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- - bb: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>build software number</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOTE: Hardware support version can be used (configurable via BOOT_CFG_HW_VER_CHECK_EN) for checking that new firmware is compatible with hardware. In case new firmware is not build for exsisting hardware, bootloader shall abort the fw upgrade procedure.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">New firmware image application version. Version is coded as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">hexadecimal format </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xMMmmddtt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, where:  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - MM: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>major software number,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- - mm: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>minor software number,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- - dd: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>develop software number,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- - bb: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>build software number</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOTE: FW version can be used (configurable via BOOT_CFG_FW_VER_CHECK_EN) for checking application compatibility with bootloader. In case bootloader do not support given application version it shall abort the fw upgrade procedure.</t>
-    </r>
-  </si>
-  <si>
     <t>INVALID REQUEST ERROR RESPONSE</t>
   </si>
   <si>
@@ -2542,6 +1793,1177 @@
       </rPr>
       <t>NOTE: Validation of new fw image placed in microcontroller internal flash is based on CRC checksum.</t>
     </r>
+  </si>
+  <si>
+    <t>Information command</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Command type
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Connect</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x11</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Connect response</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x20</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prepare</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x21</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prepare response</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x30</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flash data</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x31</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flash data response</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Exit (jump to application)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x41:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Exit response
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xA0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Information command
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xA1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Information response command</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>other values</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ignore</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>0xA0</t>
+  </si>
+  <si>
+    <t>Information response command</t>
+  </si>
+  <si>
+    <t>Bootloader version</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CRC-8 calculations based on following fields: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Source
+ - Command
+ - Status
+ - Length
+ - Bootloader version</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">New firmware image application version. Version is coded as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">hexadecimal format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xMMmmddtt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, where:  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - MM: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>major software number,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - mm: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>minor software number,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - dd: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>develop software number,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - tt: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test software number</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE: FW version can be used (configurable via BOOT_CFG_FW_VER_CHECK_EN) for checking application compatibility with bootloader. In case bootloader do not support given application version it shall abort the fw upgrade procedure.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">New firmware image hardware support version. Version is coded as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">hexadecimal format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xMMmmddtt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, where:  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - MM: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>major software number,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - mm: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>minor software number,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - dd: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>develop software number,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - tt: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test software number</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE: Hardware support version can be used (configurable via BOOT_CFG_HW_VER_CHECK_EN) for checking that new firmware is compatible with hardware. In case new firmware is not build for exsisting hardware, bootloader shall abort the fw upgrade procedure.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">New firmware image hardware support version. Version is coded as hexadecimal format 0xMMmmddtt, where:  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MM</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: major software number,
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mm</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: minor software number,
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: develop software number,
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tt</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: test software number</t>
+    </r>
+  </si>
+  <si>
+    <t>0xA1</t>
+  </si>
+  <si>
+    <t>0x37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information command shall be generated by Bootloader Manager (pc app) in order to acquire bootloader FW version. </t>
+  </si>
+  <si>
+    <r>
+      <t>On receip of that command bootloader shall evaluate command and response according to:
+ 1. If bootloader is not in "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IDLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" state, then it shall return "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Invalid request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" error,
+ 2. If bootloader is in "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IDLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" state, then it shall return with "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Information response</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" command</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Information response command is being generated by Bootloader (embedded) on reception of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> command.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exit response command is being generated by Bootloader (embedded) on reception of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> command.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prepare response command is being generated by Bootloader (embedded) on reception of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prepare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> command.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Connect Response command is being generated by Bootloader (embedded) on reception of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Connect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> command.</t>
+    </r>
+  </si>
+  <si>
+    <t>On receip of that command Bootloader Manager (PC app) shall evaluate command and response according to:
+ 1. If response is "OK", then bootloader information can be obtain
+ 2. If response is not "OK", then FW upgrade procudere do not follow bootloader sequence</t>
+  </si>
+  <si>
+    <t>0x29</t>
   </si>
 </sst>
 </file>
@@ -3194,7 +3616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3504,6 +3926,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4114,10 +4548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC1FC0B-6045-46A4-BC27-706096C9D78D}">
-  <dimension ref="A2:AD139"/>
+  <dimension ref="A2:AD168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4156,7 +4590,7 @@
     </row>
     <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="98" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C3" s="97"/>
       <c r="D3" s="97"/>
@@ -4429,7 +4863,7 @@
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="95" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="E18" s="92"/>
       <c r="F18" s="92"/>
@@ -4444,7 +4878,7 @@
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="110" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E19" s="93"/>
       <c r="F19" s="93"/>
@@ -4474,7 +4908,7 @@
       </c>
       <c r="C21" s="53"/>
       <c r="D21" s="99" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E21" s="87"/>
       <c r="F21" s="87"/>
@@ -4606,7 +5040,7 @@
         <v>39</v>
       </c>
       <c r="J29" s="101" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4640,7 +5074,7 @@
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E33" s="60"/>
       <c r="F33" s="60"/>
@@ -4664,7 +5098,7 @@
       </c>
       <c r="C34" s="53"/>
       <c r="D34" s="54" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E34" s="54"/>
       <c r="F34" s="54"/>
@@ -4724,7 +5158,7 @@
       <c r="I39" s="112"/>
       <c r="J39" s="112"/>
       <c r="L39" s="111" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M39" s="111"/>
       <c r="N39" s="111"/>
@@ -4889,7 +5323,7 @@
         <v>39</v>
       </c>
       <c r="J43" s="101" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>17</v>
@@ -4916,7 +5350,7 @@
         <v>39</v>
       </c>
       <c r="T43" s="101" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4949,8 +5383,8 @@
         <v>69</v>
       </c>
       <c r="C46" s="59"/>
-      <c r="D46" s="60" t="s">
-        <v>81</v>
+      <c r="D46" s="102" t="s">
+        <v>139</v>
       </c>
       <c r="E46" s="60"/>
       <c r="F46" s="60"/>
@@ -4974,7 +5408,7 @@
       </c>
       <c r="C47" s="53"/>
       <c r="D47" s="54" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E47" s="54"/>
       <c r="F47" s="54"/>
@@ -5139,19 +5573,19 @@
         <v>34</v>
       </c>
       <c r="K54" s="79" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L54" s="80"/>
       <c r="M54" s="80"/>
       <c r="N54" s="80"/>
       <c r="O54" s="81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="R54" s="81"/>
       <c r="S54" s="82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T54" s="82"/>
       <c r="U54" s="82"/>
@@ -5177,7 +5611,7 @@
         <v>39</v>
       </c>
       <c r="H55" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I55" s="25" t="s">
         <v>39</v>
@@ -5186,40 +5620,40 @@
         <v>35</v>
       </c>
       <c r="K55" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="L55" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="L55" s="32" t="s">
+      <c r="M55" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="M55" s="32" t="s">
+      <c r="N55" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N55" s="32" t="s">
-        <v>75</v>
-      </c>
       <c r="O55" s="33" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="P55" s="33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="Q55" s="33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="R55" s="33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="S55" s="34" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="T55" s="34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="U55" s="34" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="V55" s="35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5253,7 +5687,7 @@
       </c>
       <c r="C58" s="59"/>
       <c r="D58" s="102" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E58" s="60"/>
       <c r="F58" s="60"/>
@@ -5273,11 +5707,11 @@
     </row>
     <row r="59" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C59" s="91"/>
       <c r="D59" s="103" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E59" s="104"/>
       <c r="F59" s="104"/>
@@ -5297,11 +5731,11 @@
     </row>
     <row r="60" spans="1:25" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" s="91"/>
       <c r="D60" s="103" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="E60" s="104"/>
       <c r="F60" s="104"/>
@@ -5321,11 +5755,11 @@
     </row>
     <row r="61" spans="1:25" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="106" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="107"/>
       <c r="D61" s="54" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="E61" s="54"/>
       <c r="F61" s="54"/>
@@ -5374,7 +5808,7 @@
       </c>
       <c r="C64" s="59"/>
       <c r="D64" s="60" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E64" s="60"/>
       <c r="F64" s="60"/>
@@ -5398,7 +5832,7 @@
       </c>
       <c r="C65" s="53"/>
       <c r="D65" s="54" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E65" s="54"/>
       <c r="F65" s="54"/>
@@ -5458,7 +5892,7 @@
       <c r="I70" s="112"/>
       <c r="J70" s="112"/>
       <c r="L70" s="111" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M70" s="111"/>
       <c r="N70" s="111"/>
@@ -5469,7 +5903,7 @@
       <c r="S70" s="111"/>
       <c r="T70" s="111"/>
       <c r="V70" s="111" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="W70" s="111"/>
       <c r="X70" s="111"/>
@@ -5695,7 +6129,7 @@
         <v>39</v>
       </c>
       <c r="J74" s="101" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L74" s="12" t="s">
         <v>17</v>
@@ -5722,7 +6156,7 @@
         <v>39</v>
       </c>
       <c r="T74" s="101" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="V74" s="12" t="s">
         <v>17</v>
@@ -5749,12 +6183,12 @@
         <v>39</v>
       </c>
       <c r="AD74" s="101" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L76" s="111" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="M76" s="111"/>
       <c r="N76" s="111"/>
@@ -5765,7 +6199,7 @@
       <c r="S76" s="111"/>
       <c r="T76" s="111"/>
       <c r="V76" s="111" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="W76" s="111"/>
       <c r="X76" s="111"/>
@@ -5930,7 +6364,7 @@
         <v>39</v>
       </c>
       <c r="T80" s="101" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="V80" s="12" t="s">
         <v>17</v>
@@ -5957,7 +6391,7 @@
         <v>39</v>
       </c>
       <c r="AD80" s="101" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5990,8 +6424,8 @@
         <v>69</v>
       </c>
       <c r="C84" s="59"/>
-      <c r="D84" s="60" t="s">
-        <v>82</v>
+      <c r="D84" s="102" t="s">
+        <v>138</v>
       </c>
       <c r="E84" s="60"/>
       <c r="F84" s="60"/>
@@ -6015,7 +6449,7 @@
       </c>
       <c r="C85" s="53"/>
       <c r="D85" s="54" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E85" s="54"/>
       <c r="F85" s="54"/>
@@ -6226,7 +6660,7 @@
       </c>
       <c r="C96" s="59"/>
       <c r="D96" s="102" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E96" s="60"/>
       <c r="F96" s="60"/>
@@ -6250,7 +6684,7 @@
       </c>
       <c r="C97" s="109"/>
       <c r="D97" s="102" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E97" s="60"/>
       <c r="F97" s="60"/>
@@ -6299,7 +6733,7 @@
       </c>
       <c r="C100" s="59"/>
       <c r="D100" s="60" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E100" s="60"/>
       <c r="F100" s="60"/>
@@ -6323,7 +6757,7 @@
       </c>
       <c r="C101" s="53"/>
       <c r="D101" s="54" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E101" s="54"/>
       <c r="F101" s="54"/>
@@ -6383,7 +6817,7 @@
       <c r="I106" s="112"/>
       <c r="J106" s="112"/>
       <c r="L106" s="111" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M106" s="111"/>
       <c r="N106" s="111"/>
@@ -6620,7 +7054,7 @@
         <v>39</v>
       </c>
       <c r="J110" s="101" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="L110" s="12" t="s">
         <v>17</v>
@@ -6647,7 +7081,7 @@
         <v>39</v>
       </c>
       <c r="T110" s="101" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="V110" s="12" t="s">
         <v>17</v>
@@ -6708,7 +7142,7 @@
       </c>
       <c r="C113" s="59"/>
       <c r="D113" s="102" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E113" s="60"/>
       <c r="F113" s="60"/>
@@ -6732,7 +7166,7 @@
       </c>
       <c r="C114" s="53"/>
       <c r="D114" s="54" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E114" s="54"/>
       <c r="F114" s="54"/>
@@ -6873,7 +7307,7 @@
         <v>39</v>
       </c>
       <c r="J122" s="101" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6907,7 +7341,7 @@
       </c>
       <c r="C125" s="59"/>
       <c r="D125" s="102" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E125" s="60"/>
       <c r="F125" s="60"/>
@@ -6931,7 +7365,7 @@
       </c>
       <c r="C126" s="53"/>
       <c r="D126" s="54" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E126" s="54"/>
       <c r="F126" s="54"/>
@@ -6991,7 +7425,7 @@
       <c r="I131" s="112"/>
       <c r="J131" s="112"/>
       <c r="L131" s="111" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M131" s="111"/>
       <c r="N131" s="111"/>
@@ -7002,7 +7436,7 @@
       <c r="S131" s="111"/>
       <c r="T131" s="111"/>
       <c r="V131" s="111" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="W131" s="111"/>
       <c r="X131" s="111"/>
@@ -7228,7 +7662,7 @@
         <v>39</v>
       </c>
       <c r="J135" s="101" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="L135" s="12" t="s">
         <v>17</v>
@@ -7255,7 +7689,7 @@
         <v>39</v>
       </c>
       <c r="T135" s="101" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="V135" s="12" t="s">
         <v>17</v>
@@ -7273,7 +7707,7 @@
         <v>65</v>
       </c>
       <c r="AA135" s="19" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="AB135" s="25" t="s">
         <v>39</v>
@@ -7282,7 +7716,7 @@
         <v>39</v>
       </c>
       <c r="AD135" s="101" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="136" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7315,8 +7749,8 @@
         <v>69</v>
       </c>
       <c r="C138" s="59"/>
-      <c r="D138" s="60" t="s">
-        <v>85</v>
+      <c r="D138" s="102" t="s">
+        <v>137</v>
       </c>
       <c r="E138" s="60"/>
       <c r="F138" s="60"/>
@@ -7340,7 +7774,7 @@
       </c>
       <c r="C139" s="53"/>
       <c r="D139" s="54" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E139" s="54"/>
       <c r="F139" s="54"/>
@@ -7358,8 +7792,663 @@
       <c r="R139" s="54"/>
       <c r="S139" s="55"/>
     </row>
+    <row r="142" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A142" s="30"/>
+      <c r="B142" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C142" s="62"/>
+      <c r="D142" s="62"/>
+      <c r="E142" s="62"/>
+      <c r="F142" s="62"/>
+      <c r="G142" s="62"/>
+      <c r="H142" s="62"/>
+      <c r="I142" s="62"/>
+      <c r="J142" s="62"/>
+      <c r="K142" s="62"/>
+      <c r="L142" s="62"/>
+      <c r="M142" s="62"/>
+      <c r="N142" s="62"/>
+      <c r="O142" s="62"/>
+      <c r="P142" s="62"/>
+      <c r="Q142" s="62"/>
+      <c r="R142" s="62"/>
+      <c r="S142" s="62"/>
+      <c r="T142" s="62"/>
+      <c r="U142" s="62"/>
+      <c r="V142" s="62"/>
+      <c r="W142" s="62"/>
+      <c r="X142" s="62"/>
+      <c r="Y142" s="62"/>
+    </row>
+    <row r="143" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B144" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="13">
+        <v>0</v>
+      </c>
+      <c r="D144" s="13">
+        <v>1</v>
+      </c>
+      <c r="E144" s="13">
+        <v>2</v>
+      </c>
+      <c r="F144" s="13">
+        <v>3</v>
+      </c>
+      <c r="G144" s="13">
+        <v>4</v>
+      </c>
+      <c r="H144" s="13">
+        <v>5</v>
+      </c>
+      <c r="I144" s="13">
+        <v>6</v>
+      </c>
+      <c r="J144" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B145" s="15"/>
+      <c r="C145" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="65"/>
+      <c r="E145" s="65"/>
+      <c r="F145" s="65"/>
+      <c r="G145" s="65"/>
+      <c r="H145" s="65"/>
+      <c r="I145" s="65"/>
+      <c r="J145" s="66"/>
+    </row>
+    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B146" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D146" s="68"/>
+      <c r="E146" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F146" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G146" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H146" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="I146" s="69"/>
+      <c r="J146" s="100" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="147" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C147" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D147" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E147" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F147" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G147" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H147" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I147" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J147" s="101" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B149" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C149" s="64"/>
+      <c r="D149" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E149" s="56"/>
+      <c r="F149" s="56"/>
+      <c r="G149" s="56"/>
+      <c r="H149" s="56"/>
+      <c r="I149" s="56"/>
+      <c r="J149" s="56"/>
+      <c r="K149" s="56"/>
+      <c r="L149" s="56"/>
+      <c r="M149" s="56"/>
+      <c r="N149" s="56"/>
+      <c r="O149" s="56"/>
+      <c r="P149" s="56"/>
+      <c r="Q149" s="56"/>
+      <c r="R149" s="56"/>
+      <c r="S149" s="57"/>
+    </row>
+    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B150" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C150" s="59"/>
+      <c r="D150" s="102" t="s">
+        <v>134</v>
+      </c>
+      <c r="E150" s="60"/>
+      <c r="F150" s="60"/>
+      <c r="G150" s="60"/>
+      <c r="H150" s="60"/>
+      <c r="I150" s="60"/>
+      <c r="J150" s="60"/>
+      <c r="K150" s="60"/>
+      <c r="L150" s="60"/>
+      <c r="M150" s="60"/>
+      <c r="N150" s="60"/>
+      <c r="O150" s="60"/>
+      <c r="P150" s="60"/>
+      <c r="Q150" s="60"/>
+      <c r="R150" s="60"/>
+      <c r="S150" s="61"/>
+    </row>
+    <row r="151" spans="1:25" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C151" s="53"/>
+      <c r="D151" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="E151" s="54"/>
+      <c r="F151" s="54"/>
+      <c r="G151" s="54"/>
+      <c r="H151" s="54"/>
+      <c r="I151" s="54"/>
+      <c r="J151" s="54"/>
+      <c r="K151" s="54"/>
+      <c r="L151" s="54"/>
+      <c r="M151" s="54"/>
+      <c r="N151" s="54"/>
+      <c r="O151" s="54"/>
+      <c r="P151" s="54"/>
+      <c r="Q151" s="54"/>
+      <c r="R151" s="54"/>
+      <c r="S151" s="55"/>
+    </row>
+    <row r="154" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A154" s="30"/>
+      <c r="B154" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C154" s="62"/>
+      <c r="D154" s="62"/>
+      <c r="E154" s="62"/>
+      <c r="F154" s="62"/>
+      <c r="G154" s="62"/>
+      <c r="H154" s="62"/>
+      <c r="I154" s="62"/>
+      <c r="J154" s="62"/>
+      <c r="K154" s="62"/>
+      <c r="L154" s="62"/>
+      <c r="M154" s="62"/>
+      <c r="N154" s="62"/>
+      <c r="O154" s="62"/>
+      <c r="P154" s="62"/>
+      <c r="Q154" s="62"/>
+      <c r="R154" s="62"/>
+      <c r="S154" s="62"/>
+      <c r="T154" s="62"/>
+      <c r="U154" s="62"/>
+      <c r="V154" s="62"/>
+      <c r="W154" s="62"/>
+      <c r="X154" s="62"/>
+      <c r="Y154" s="62"/>
+    </row>
+    <row r="156" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="C156" s="112"/>
+      <c r="D156" s="112"/>
+      <c r="E156" s="112"/>
+      <c r="F156" s="112"/>
+      <c r="G156" s="112"/>
+      <c r="H156" s="112"/>
+      <c r="I156" s="112"/>
+      <c r="J156" s="112"/>
+      <c r="K156" s="112"/>
+      <c r="L156" s="112"/>
+      <c r="M156" s="112"/>
+      <c r="N156" s="112"/>
+      <c r="P156" s="111" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q156" s="111"/>
+      <c r="R156" s="111"/>
+      <c r="S156" s="111"/>
+      <c r="T156" s="111"/>
+      <c r="U156" s="111"/>
+      <c r="V156" s="111"/>
+      <c r="W156" s="111"/>
+      <c r="X156" s="111"/>
+    </row>
+    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B157" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" s="13">
+        <v>0</v>
+      </c>
+      <c r="D157" s="13">
+        <v>1</v>
+      </c>
+      <c r="E157" s="13">
+        <v>2</v>
+      </c>
+      <c r="F157" s="13">
+        <v>3</v>
+      </c>
+      <c r="G157" s="13">
+        <v>4</v>
+      </c>
+      <c r="H157" s="13">
+        <v>5</v>
+      </c>
+      <c r="I157" s="13">
+        <v>6</v>
+      </c>
+      <c r="J157" s="14">
+        <v>7</v>
+      </c>
+      <c r="K157" s="26">
+        <v>8</v>
+      </c>
+      <c r="L157" s="13">
+        <v>9</v>
+      </c>
+      <c r="M157" s="13">
+        <v>10</v>
+      </c>
+      <c r="N157" s="14">
+        <v>11</v>
+      </c>
+      <c r="P157" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q157" s="13">
+        <v>0</v>
+      </c>
+      <c r="R157" s="13">
+        <v>1</v>
+      </c>
+      <c r="S157" s="13">
+        <v>2</v>
+      </c>
+      <c r="T157" s="13">
+        <v>3</v>
+      </c>
+      <c r="U157" s="13">
+        <v>4</v>
+      </c>
+      <c r="V157" s="13">
+        <v>5</v>
+      </c>
+      <c r="W157" s="13">
+        <v>6</v>
+      </c>
+      <c r="X157" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B158" s="15"/>
+      <c r="C158" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D158" s="65"/>
+      <c r="E158" s="65"/>
+      <c r="F158" s="65"/>
+      <c r="G158" s="65"/>
+      <c r="H158" s="65"/>
+      <c r="I158" s="65"/>
+      <c r="J158" s="66"/>
+      <c r="K158" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="L158" s="71"/>
+      <c r="M158" s="71"/>
+      <c r="N158" s="72"/>
+      <c r="P158" s="15"/>
+      <c r="Q158" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="R158" s="65"/>
+      <c r="S158" s="65"/>
+      <c r="T158" s="65"/>
+      <c r="U158" s="65"/>
+      <c r="V158" s="65"/>
+      <c r="W158" s="65"/>
+      <c r="X158" s="66"/>
+    </row>
+    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B159" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C159" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D159" s="68"/>
+      <c r="E159" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F159" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G159" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H159" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="I159" s="69"/>
+      <c r="J159" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="K159" s="113" t="s">
+        <v>127</v>
+      </c>
+      <c r="L159" s="81"/>
+      <c r="M159" s="81"/>
+      <c r="N159" s="114"/>
+      <c r="P159" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q159" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="R159" s="68"/>
+      <c r="S159" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="T159" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="U159" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="V159" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="W159" s="69"/>
+      <c r="X159" s="100" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="160" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D160" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E160" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F160" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G160" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H160" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I160" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J160" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="K160" s="115" t="s">
+        <v>89</v>
+      </c>
+      <c r="L160" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="M160" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="N160" s="116" t="s">
+        <v>92</v>
+      </c>
+      <c r="P160" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q160" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R160" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S160" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T160" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="U160" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="V160" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="W160" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="X160" s="101" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="161" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B162" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C162" s="64"/>
+      <c r="D162" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E162" s="56"/>
+      <c r="F162" s="56"/>
+      <c r="G162" s="56"/>
+      <c r="H162" s="56"/>
+      <c r="I162" s="56"/>
+      <c r="J162" s="56"/>
+      <c r="K162" s="56"/>
+      <c r="L162" s="56"/>
+      <c r="M162" s="56"/>
+      <c r="N162" s="56"/>
+      <c r="O162" s="56"/>
+      <c r="P162" s="56"/>
+      <c r="Q162" s="56"/>
+      <c r="R162" s="56"/>
+      <c r="S162" s="57"/>
+    </row>
+    <row r="163" spans="2:19" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C163" s="59"/>
+      <c r="D163" s="102" t="s">
+        <v>128</v>
+      </c>
+      <c r="E163" s="60"/>
+      <c r="F163" s="60"/>
+      <c r="G163" s="60"/>
+      <c r="H163" s="60"/>
+      <c r="I163" s="60"/>
+      <c r="J163" s="60"/>
+      <c r="K163" s="60"/>
+      <c r="L163" s="60"/>
+      <c r="M163" s="60"/>
+      <c r="N163" s="60"/>
+      <c r="O163" s="60"/>
+      <c r="P163" s="60"/>
+      <c r="Q163" s="60"/>
+      <c r="R163" s="60"/>
+      <c r="S163" s="61"/>
+    </row>
+    <row r="164" spans="2:19" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="C164" s="109"/>
+      <c r="D164" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="E164" s="60"/>
+      <c r="F164" s="60"/>
+      <c r="G164" s="60"/>
+      <c r="H164" s="60"/>
+      <c r="I164" s="60"/>
+      <c r="J164" s="60"/>
+      <c r="K164" s="60"/>
+      <c r="L164" s="60"/>
+      <c r="M164" s="60"/>
+      <c r="N164" s="60"/>
+      <c r="O164" s="60"/>
+      <c r="P164" s="60"/>
+      <c r="Q164" s="60"/>
+      <c r="R164" s="60"/>
+      <c r="S164" s="61"/>
+    </row>
+    <row r="165" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B166" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C166" s="64"/>
+      <c r="D166" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E166" s="56"/>
+      <c r="F166" s="56"/>
+      <c r="G166" s="56"/>
+      <c r="H166" s="56"/>
+      <c r="I166" s="56"/>
+      <c r="J166" s="56"/>
+      <c r="K166" s="56"/>
+      <c r="L166" s="56"/>
+      <c r="M166" s="56"/>
+      <c r="N166" s="56"/>
+      <c r="O166" s="56"/>
+      <c r="P166" s="56"/>
+      <c r="Q166" s="56"/>
+      <c r="R166" s="56"/>
+      <c r="S166" s="57"/>
+    </row>
+    <row r="167" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B167" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C167" s="59"/>
+      <c r="D167" s="102" t="s">
+        <v>136</v>
+      </c>
+      <c r="E167" s="60"/>
+      <c r="F167" s="60"/>
+      <c r="G167" s="60"/>
+      <c r="H167" s="60"/>
+      <c r="I167" s="60"/>
+      <c r="J167" s="60"/>
+      <c r="K167" s="60"/>
+      <c r="L167" s="60"/>
+      <c r="M167" s="60"/>
+      <c r="N167" s="60"/>
+      <c r="O167" s="60"/>
+      <c r="P167" s="60"/>
+      <c r="Q167" s="60"/>
+      <c r="R167" s="60"/>
+      <c r="S167" s="61"/>
+    </row>
+    <row r="168" spans="2:19" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C168" s="53"/>
+      <c r="D168" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="E168" s="54"/>
+      <c r="F168" s="54"/>
+      <c r="G168" s="54"/>
+      <c r="H168" s="54"/>
+      <c r="I168" s="54"/>
+      <c r="J168" s="54"/>
+      <c r="K168" s="54"/>
+      <c r="L168" s="54"/>
+      <c r="M168" s="54"/>
+      <c r="N168" s="54"/>
+      <c r="O168" s="54"/>
+      <c r="P168" s="54"/>
+      <c r="Q168" s="54"/>
+      <c r="R168" s="54"/>
+      <c r="S168" s="55"/>
+    </row>
   </sheetData>
-  <mergeCells count="164">
+  <mergeCells count="197">
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="D168:S168"/>
+    <mergeCell ref="P156:X156"/>
+    <mergeCell ref="Q158:X158"/>
+    <mergeCell ref="Q159:R159"/>
+    <mergeCell ref="V159:W159"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:S162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="D163:S163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="D164:S164"/>
+    <mergeCell ref="B156:N156"/>
+    <mergeCell ref="B154:Y154"/>
+    <mergeCell ref="C158:J158"/>
+    <mergeCell ref="K158:N158"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="H159:I159"/>
+    <mergeCell ref="K159:N159"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="D166:S166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="D167:S167"/>
+    <mergeCell ref="B142:Y142"/>
+    <mergeCell ref="C145:J145"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="H146:I146"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="D149:S149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:S150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="D151:S151"/>
     <mergeCell ref="V70:AD70"/>
     <mergeCell ref="W72:AD72"/>
     <mergeCell ref="W73:X73"/>

</xml_diff>

<commit_message>
- updated bootloader specifications
</commit_message>
<xml_diff>
--- a/doc/Bootloader_Interface_Specifications.xlsx
+++ b/doc/Bootloader_Interface_Specifications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\ORDERBOB_ECS__2023\SOFTWARE\MASTER_SOURCE\ECS_Bootloader\OrderBob\middleware\boot\boot\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SELTRON\zigamiklosic\Personal\HomeWork\ECS_Bootloader\OrderBob\middleware\boot\boot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD11124E-723D-4DB6-A4CC-DC5CDF32375A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7E5CC1-6FB9-4AB6-B967-6038311E1842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -480,137 +480,6 @@
  - Binary Interface</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRC checksum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of following fields:
- - Source
- - Command
- - Status
- - Length
- - Payload (in case of "</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Flash data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" command)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">CRC-8 calculation details:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Polynom:</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 0x07</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (CRC-8-CCITT)
- - Custom seed: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB6</t>
-    </r>
-  </si>
-  <si>
-    <t>0xAF</t>
-  </si>
-  <si>
-    <t>0x67</t>
-  </si>
-  <si>
-    <t>0xB1</t>
-  </si>
-  <si>
     <t>New FW size</t>
   </si>
   <si>
@@ -672,12 +541,6 @@
     <t>INVALID REQUEST ERROR RESPONSE</t>
   </si>
   <si>
-    <t>0xCE</t>
-  </si>
-  <si>
-    <t>0x18</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">CRC-8 calculations based on following fields: 
 </t>
@@ -1029,12 +892,6 @@
     <t>Flash Data response command is being generated by Bootloader (embedded) after write binary data to flash. Writing to flash is triggered on reception of Flash Data command.</t>
   </si>
   <si>
-    <t>0xA9</t>
-  </si>
-  <si>
-    <t>0x53</t>
-  </si>
-  <si>
     <r>
       <t>Exit command shall be generated after final "</t>
     </r>
@@ -1121,12 +978,6 @@
   </si>
   <si>
     <t>0x9B</t>
-  </si>
-  <si>
-    <t>0xF0</t>
-  </si>
-  <si>
-    <t>0x7F</t>
   </si>
   <si>
     <t>FIRMWARE IMAGE SIZE ERROR RESPONSE</t>
@@ -1626,15 +1477,6 @@
       <t xml:space="preserve">" status
 </t>
     </r>
-  </si>
-  <si>
-    <t>0x6C</t>
-  </si>
-  <si>
-    <t>0x8D</t>
-  </si>
-  <si>
-    <t>0x9F</t>
   </si>
   <si>
     <t>0x4D</t>
@@ -2744,9 +2586,6 @@
     <t>0xA1</t>
   </si>
   <si>
-    <t>0x37</t>
-  </si>
-  <si>
     <t xml:space="preserve">Information command shall be generated by Bootloader Manager (pc app) in order to acquire bootloader FW version. </t>
   </si>
   <si>
@@ -2963,19 +2802,201 @@
  2. If response is not "OK", then FW upgrade procudere do not follow bootloader sequence</t>
   </si>
   <si>
-    <t>0x29</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRC checksum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of following fields:
+ - Source
+ - Command
+ - Status
+ - Length
+ - Payload (in case of "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flash data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" command)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CRC-8 calculation details:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Polynom:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0x07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (CRC-8-CCITT)
+ - Custom seed: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - Message CRC calculation shall be done as:
+</t>
+    </r>
+  </si>
+  <si>
+    <t>0x5A</t>
+  </si>
+  <si>
+    <t>0x54</t>
+  </si>
+  <si>
+    <t>0xCA</t>
+  </si>
+  <si>
+    <t>0xC4</t>
+  </si>
+  <si>
+    <t>0xBA</t>
+  </si>
+  <si>
+    <t>0x2A</t>
+  </si>
+  <si>
+    <t>0xF2</t>
+  </si>
+  <si>
+    <t>0xB4</t>
+  </si>
+  <si>
+    <t>0xA6</t>
+  </si>
+  <si>
+    <t>0x2C</t>
+  </si>
+  <si>
+    <t>0xED</t>
+  </si>
+  <si>
+    <t>0xE3</t>
+  </si>
+  <si>
+    <t>0xEA</t>
+  </si>
+  <si>
+    <t>0x82</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3636,135 +3657,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3773,183 +3816,161 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4084,6 +4105,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>33615</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2229970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>637561</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4807324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D8ED732-6647-DCF0-157E-A1CD13BAF1EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1983439" y="12987617"/>
+          <a:ext cx="4638063" cy="2577354"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4368,19 +4433,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -4393,14 +4458,14 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="49"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -4412,20 +4477,20 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="55"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="52"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
@@ -4436,7 +4501,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="40"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
@@ -4447,7 +4512,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="41"/>
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
@@ -4458,7 +4523,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="52"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="41"/>
       <c r="G9" s="41"/>
       <c r="H9" s="41"/>
@@ -4469,7 +4534,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="52"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="41"/>
       <c r="G10" s="41"/>
       <c r="H10" s="41"/>
@@ -4480,7 +4545,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="52"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="41"/>
       <c r="G11" s="41"/>
       <c r="H11" s="41"/>
@@ -4491,7 +4556,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="52"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="41"/>
       <c r="G12" s="41"/>
       <c r="H12" s="41"/>
@@ -4502,7 +4567,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="52"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="41"/>
       <c r="G13" s="41"/>
       <c r="H13" s="41"/>
@@ -4513,7 +4578,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="52"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
@@ -4524,15 +4589,21 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="55"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -4541,12 +4612,6 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4557,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC1FC0B-6045-46A4-BC27-706096C9D78D}">
   <dimension ref="A2:AD168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4568,60 +4633,60 @@
   <sheetData>
     <row r="2" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="30"/>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
     </row>
     <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
-      <c r="T3" s="94"/>
-      <c r="U3" s="94"/>
-      <c r="V3" s="94"/>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="94"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="106"/>
+      <c r="O3" s="106"/>
+      <c r="P3" s="106"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="106"/>
+      <c r="U3" s="106"/>
+      <c r="V3" s="106"/>
+      <c r="W3" s="106"/>
+      <c r="X3" s="106"/>
+      <c r="Y3" s="106"/>
     </row>
     <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -4673,53 +4738,53 @@
     </row>
     <row r="6" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="96" t="s">
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="97"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="90"/>
     </row>
     <row r="8" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="30"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="78"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="78"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="75"/>
+      <c r="V8" s="75"/>
+      <c r="W8" s="75"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="75"/>
     </row>
     <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -4753,29 +4818,29 @@
     </row>
     <row r="11" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="62"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65" t="s">
+      <c r="D12" s="61"/>
+      <c r="E12" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="65"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="20" t="s">
         <v>23</v>
       </c>
@@ -4820,10 +4885,10 @@
     </row>
     <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="68" t="s">
         <v>4</v>
       </c>
@@ -4839,119 +4904,119 @@
         <v>20</v>
       </c>
       <c r="C16" s="71"/>
-      <c r="D16" s="110" t="s">
+      <c r="D16" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="103"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="95"/>
     </row>
     <row r="17" spans="1:25" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="70" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="71"/>
-      <c r="D17" s="104" t="s">
+      <c r="D17" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="92"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="100"/>
     </row>
     <row r="18" spans="1:25" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="70" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="71"/>
-      <c r="D18" s="105" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="106"/>
+      <c r="D18" s="101" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="102"/>
     </row>
     <row r="19" spans="1:25" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="70" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="71"/>
-      <c r="D19" s="90" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="92"/>
+      <c r="D19" s="104" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="100"/>
     </row>
     <row r="20" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="88" t="s">
+      <c r="B20" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="89"/>
-      <c r="D20" s="101" t="s">
+      <c r="C20" s="97"/>
+      <c r="D20" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="102"/>
-      <c r="J20" s="103"/>
-    </row>
-    <row r="21" spans="1:25" ht="167.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="56" t="s">
+      <c r="E20" s="94"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="95"/>
+    </row>
+    <row r="21" spans="1:25" ht="381.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="98" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="100"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="119" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="92"/>
     </row>
     <row r="24" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="30"/>
-      <c r="B24" s="78" t="s">
+      <c r="B24" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="78"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="78"/>
-      <c r="V24" s="78"/>
-      <c r="W24" s="78"/>
-      <c r="X24" s="78"/>
-      <c r="Y24" s="78"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="75"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="75"/>
+      <c r="T24" s="75"/>
+      <c r="U24" s="75"/>
+      <c r="V24" s="75"/>
+      <c r="W24" s="75"/>
+      <c r="X24" s="75"/>
+      <c r="Y24" s="75"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -4985,29 +5050,29 @@
     </row>
     <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="62"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="59"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="65"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="20" t="s">
         <v>23</v>
       </c>
@@ -5047,15 +5112,15 @@
         <v>39</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="67"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="68" t="s">
         <v>4</v>
       </c>
@@ -5100,90 +5165,90 @@
       <c r="S33" s="74"/>
     </row>
     <row r="34" spans="1:30" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="59"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
+      <c r="S34" s="67"/>
     </row>
     <row r="37" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A37" s="30"/>
-      <c r="B37" s="78" t="s">
+      <c r="B37" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="78"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="78"/>
-      <c r="O37" s="78"/>
-      <c r="P37" s="78"/>
-      <c r="Q37" s="78"/>
-      <c r="R37" s="78"/>
-      <c r="S37" s="78"/>
-      <c r="T37" s="78"/>
-      <c r="U37" s="78"/>
-      <c r="V37" s="78"/>
-      <c r="W37" s="78"/>
-      <c r="X37" s="78"/>
-      <c r="Y37" s="78"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="75"/>
+      <c r="U37" s="75"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="75"/>
+      <c r="X37" s="75"/>
+      <c r="Y37" s="75"/>
     </row>
     <row r="39" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="77" t="s">
+      <c r="B39" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
-      <c r="L39" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="M39" s="60"/>
-      <c r="N39" s="60"/>
-      <c r="O39" s="60"/>
-      <c r="P39" s="60"/>
-      <c r="Q39" s="60"/>
-      <c r="R39" s="60"/>
-      <c r="S39" s="60"/>
-      <c r="T39" s="60"/>
-      <c r="V39" s="119"/>
-      <c r="W39" s="119"/>
-      <c r="X39" s="119"/>
-      <c r="Y39" s="119"/>
-      <c r="Z39" s="119"/>
-      <c r="AA39" s="119"/>
-      <c r="AB39" s="119"/>
-      <c r="AC39" s="119"/>
-      <c r="AD39" s="119"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="78"/>
+      <c r="L39" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="M39" s="79"/>
+      <c r="N39" s="79"/>
+      <c r="O39" s="79"/>
+      <c r="P39" s="79"/>
+      <c r="Q39" s="79"/>
+      <c r="R39" s="79"/>
+      <c r="S39" s="79"/>
+      <c r="T39" s="79"/>
+      <c r="V39" s="57"/>
+      <c r="W39" s="57"/>
+      <c r="X39" s="57"/>
+      <c r="Y39" s="57"/>
+      <c r="Z39" s="57"/>
+      <c r="AA39" s="57"/>
+      <c r="AB39" s="57"/>
+      <c r="AC39" s="57"/>
+      <c r="AD39" s="57"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
@@ -5243,40 +5308,40 @@
     </row>
     <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="15"/>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="62"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="59"/>
       <c r="L41" s="15"/>
-      <c r="M41" s="61" t="s">
+      <c r="M41" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="N41" s="61"/>
-      <c r="O41" s="61"/>
-      <c r="P41" s="61"/>
-      <c r="Q41" s="61"/>
-      <c r="R41" s="61"/>
-      <c r="S41" s="61"/>
-      <c r="T41" s="62"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="58"/>
+      <c r="R41" s="58"/>
+      <c r="S41" s="58"/>
+      <c r="T41" s="59"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="117" t="s">
+      <c r="D42" s="61"/>
+      <c r="E42" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="118"/>
+      <c r="F42" s="63"/>
       <c r="G42" s="20" t="s">
         <v>23</v>
       </c>
@@ -5292,14 +5357,14 @@
       <c r="L42" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M42" s="63" t="s">
+      <c r="M42" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="N42" s="64"/>
-      <c r="O42" s="117" t="s">
+      <c r="N42" s="61"/>
+      <c r="O42" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="P42" s="118"/>
+      <c r="P42" s="63"/>
       <c r="Q42" s="20" t="s">
         <v>23</v>
       </c>
@@ -5339,7 +5404,7 @@
         <v>39</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>17</v>
@@ -5366,15 +5431,15 @@
         <v>41</v>
       </c>
       <c r="T43" s="37" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="67"/>
+      <c r="C45" s="77"/>
       <c r="D45" s="68" t="s">
         <v>4</v>
       </c>
@@ -5400,7 +5465,7 @@
       </c>
       <c r="C46" s="71"/>
       <c r="D46" s="72" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E46" s="73"/>
       <c r="F46" s="73"/>
@@ -5419,57 +5484,57 @@
       <c r="S46" s="74"/>
     </row>
     <row r="47" spans="1:30" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
-      <c r="P47" s="58"/>
-      <c r="Q47" s="58"/>
-      <c r="R47" s="58"/>
-      <c r="S47" s="59"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="66"/>
+      <c r="L47" s="66"/>
+      <c r="M47" s="66"/>
+      <c r="N47" s="66"/>
+      <c r="O47" s="66"/>
+      <c r="P47" s="66"/>
+      <c r="Q47" s="66"/>
+      <c r="R47" s="66"/>
+      <c r="S47" s="67"/>
     </row>
     <row r="50" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A50" s="30"/>
-      <c r="B50" s="78" t="s">
+      <c r="B50" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
-      <c r="G50" s="78"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="78"/>
-      <c r="J50" s="78"/>
-      <c r="K50" s="78"/>
-      <c r="L50" s="78"/>
-      <c r="M50" s="78"/>
-      <c r="N50" s="78"/>
-      <c r="O50" s="78"/>
-      <c r="P50" s="78"/>
-      <c r="Q50" s="78"/>
-      <c r="R50" s="78"/>
-      <c r="S50" s="78"/>
-      <c r="T50" s="78"/>
-      <c r="U50" s="78"/>
-      <c r="V50" s="78"/>
-      <c r="W50" s="78"/>
-      <c r="X50" s="78"/>
-      <c r="Y50" s="78"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="75"/>
+      <c r="K50" s="75"/>
+      <c r="L50" s="75"/>
+      <c r="M50" s="75"/>
+      <c r="N50" s="75"/>
+      <c r="O50" s="75"/>
+      <c r="P50" s="75"/>
+      <c r="Q50" s="75"/>
+      <c r="R50" s="75"/>
+      <c r="S50" s="75"/>
+      <c r="T50" s="75"/>
+      <c r="U50" s="75"/>
+      <c r="V50" s="75"/>
+      <c r="W50" s="75"/>
+      <c r="X50" s="75"/>
+      <c r="Y50" s="75"/>
     </row>
     <row r="51" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
@@ -5539,43 +5604,43 @@
     </row>
     <row r="53" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="15"/>
-      <c r="C53" s="61" t="s">
+      <c r="C53" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="61"/>
-      <c r="I53" s="61"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="79" t="s">
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="L53" s="80"/>
-      <c r="M53" s="80"/>
-      <c r="N53" s="80"/>
-      <c r="O53" s="80"/>
-      <c r="P53" s="80"/>
-      <c r="Q53" s="80"/>
-      <c r="R53" s="80"/>
-      <c r="S53" s="80"/>
-      <c r="T53" s="80"/>
-      <c r="U53" s="80"/>
-      <c r="V53" s="81"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="84"/>
+      <c r="N53" s="84"/>
+      <c r="O53" s="84"/>
+      <c r="P53" s="84"/>
+      <c r="Q53" s="84"/>
+      <c r="R53" s="84"/>
+      <c r="S53" s="84"/>
+      <c r="T53" s="84"/>
+      <c r="U53" s="84"/>
+      <c r="V53" s="85"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="63" t="s">
+      <c r="C54" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="64"/>
-      <c r="E54" s="65" t="s">
+      <c r="D54" s="61"/>
+      <c r="E54" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F54" s="65"/>
+      <c r="F54" s="56"/>
       <c r="G54" s="20" t="s">
         <v>23</v>
       </c>
@@ -5588,24 +5653,24 @@
       <c r="J54" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="K54" s="111" t="s">
-        <v>87</v>
-      </c>
-      <c r="L54" s="112"/>
-      <c r="M54" s="112"/>
-      <c r="N54" s="112"/>
-      <c r="O54" s="83" t="s">
+      <c r="K54" s="107" t="s">
+        <v>83</v>
+      </c>
+      <c r="L54" s="108"/>
+      <c r="M54" s="108"/>
+      <c r="N54" s="108"/>
+      <c r="O54" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="P54" s="83"/>
-      <c r="Q54" s="83"/>
-      <c r="R54" s="83"/>
-      <c r="S54" s="113" t="s">
+      <c r="P54" s="80"/>
+      <c r="Q54" s="80"/>
+      <c r="R54" s="80"/>
+      <c r="S54" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="T54" s="113"/>
-      <c r="U54" s="113"/>
-      <c r="V54" s="114"/>
+      <c r="T54" s="81"/>
+      <c r="U54" s="81"/>
+      <c r="V54" s="82"/>
     </row>
     <row r="55" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="12" t="s">
@@ -5648,36 +5713,36 @@
         <v>74</v>
       </c>
       <c r="O55" s="33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P55" s="33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q55" s="33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R55" s="33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="S55" s="34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="T55" s="34" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="U55" s="34" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="V55" s="35" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B57" s="66" t="s">
+      <c r="B57" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="67"/>
+      <c r="C57" s="77"/>
       <c r="D57" s="68" t="s">
         <v>4</v>
       </c>
@@ -5703,7 +5768,7 @@
       </c>
       <c r="C58" s="71"/>
       <c r="D58" s="72" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E58" s="73"/>
       <c r="F58" s="73"/>
@@ -5722,83 +5787,83 @@
       <c r="S58" s="74"/>
     </row>
     <row r="59" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="88" t="s">
+      <c r="B59" s="96" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="89"/>
-      <c r="D59" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="E59" s="86"/>
-      <c r="F59" s="86"/>
-      <c r="G59" s="86"/>
-      <c r="H59" s="86"/>
-      <c r="I59" s="86"/>
-      <c r="J59" s="86"/>
-      <c r="K59" s="86"/>
-      <c r="L59" s="86"/>
-      <c r="M59" s="86"/>
-      <c r="N59" s="86"/>
-      <c r="O59" s="86"/>
-      <c r="P59" s="86"/>
-      <c r="Q59" s="86"/>
-      <c r="R59" s="86"/>
-      <c r="S59" s="87"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="109" t="s">
+        <v>89</v>
+      </c>
+      <c r="E59" s="110"/>
+      <c r="F59" s="110"/>
+      <c r="G59" s="110"/>
+      <c r="H59" s="110"/>
+      <c r="I59" s="110"/>
+      <c r="J59" s="110"/>
+      <c r="K59" s="110"/>
+      <c r="L59" s="110"/>
+      <c r="M59" s="110"/>
+      <c r="N59" s="110"/>
+      <c r="O59" s="110"/>
+      <c r="P59" s="110"/>
+      <c r="Q59" s="110"/>
+      <c r="R59" s="110"/>
+      <c r="S59" s="111"/>
     </row>
     <row r="60" spans="1:25" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="88" t="s">
+      <c r="B60" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="89"/>
-      <c r="D60" s="85" t="s">
-        <v>129</v>
-      </c>
-      <c r="E60" s="86"/>
-      <c r="F60" s="86"/>
-      <c r="G60" s="86"/>
-      <c r="H60" s="86"/>
-      <c r="I60" s="86"/>
-      <c r="J60" s="86"/>
-      <c r="K60" s="86"/>
-      <c r="L60" s="86"/>
-      <c r="M60" s="86"/>
-      <c r="N60" s="86"/>
-      <c r="O60" s="86"/>
-      <c r="P60" s="86"/>
-      <c r="Q60" s="86"/>
-      <c r="R60" s="86"/>
-      <c r="S60" s="87"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="109" t="s">
+        <v>116</v>
+      </c>
+      <c r="E60" s="110"/>
+      <c r="F60" s="110"/>
+      <c r="G60" s="110"/>
+      <c r="H60" s="110"/>
+      <c r="I60" s="110"/>
+      <c r="J60" s="110"/>
+      <c r="K60" s="110"/>
+      <c r="L60" s="110"/>
+      <c r="M60" s="110"/>
+      <c r="N60" s="110"/>
+      <c r="O60" s="110"/>
+      <c r="P60" s="110"/>
+      <c r="Q60" s="110"/>
+      <c r="R60" s="110"/>
+      <c r="S60" s="111"/>
     </row>
     <row r="61" spans="1:25" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="115" t="s">
+      <c r="B61" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="116"/>
-      <c r="D61" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
-      <c r="K61" s="58"/>
-      <c r="L61" s="58"/>
-      <c r="M61" s="58"/>
-      <c r="N61" s="58"/>
-      <c r="O61" s="58"/>
-      <c r="P61" s="58"/>
-      <c r="Q61" s="58"/>
-      <c r="R61" s="58"/>
-      <c r="S61" s="59"/>
+      <c r="C61" s="87"/>
+      <c r="D61" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="L61" s="66"/>
+      <c r="M61" s="66"/>
+      <c r="N61" s="66"/>
+      <c r="O61" s="66"/>
+      <c r="P61" s="66"/>
+      <c r="Q61" s="66"/>
+      <c r="R61" s="66"/>
+      <c r="S61" s="67"/>
     </row>
     <row r="62" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B63" s="66" t="s">
+      <c r="B63" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="67"/>
+      <c r="C63" s="77"/>
       <c r="D63" s="68" t="s">
         <v>4</v>
       </c>
@@ -5843,92 +5908,92 @@
       <c r="S64" s="74"/>
     </row>
     <row r="65" spans="1:30" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="56" t="s">
+      <c r="B65" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="57"/>
-      <c r="D65" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="58"/>
-      <c r="J65" s="58"/>
-      <c r="K65" s="58"/>
-      <c r="L65" s="58"/>
-      <c r="M65" s="58"/>
-      <c r="N65" s="58"/>
-      <c r="O65" s="58"/>
-      <c r="P65" s="58"/>
-      <c r="Q65" s="58"/>
-      <c r="R65" s="58"/>
-      <c r="S65" s="59"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="66"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="66"/>
+      <c r="H65" s="66"/>
+      <c r="I65" s="66"/>
+      <c r="J65" s="66"/>
+      <c r="K65" s="66"/>
+      <c r="L65" s="66"/>
+      <c r="M65" s="66"/>
+      <c r="N65" s="66"/>
+      <c r="O65" s="66"/>
+      <c r="P65" s="66"/>
+      <c r="Q65" s="66"/>
+      <c r="R65" s="66"/>
+      <c r="S65" s="67"/>
     </row>
     <row r="68" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A68" s="30"/>
-      <c r="B68" s="78" t="s">
+      <c r="B68" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="78"/>
-      <c r="D68" s="78"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="78"/>
-      <c r="G68" s="78"/>
-      <c r="H68" s="78"/>
-      <c r="I68" s="78"/>
-      <c r="J68" s="78"/>
-      <c r="K68" s="78"/>
-      <c r="L68" s="78"/>
-      <c r="M68" s="78"/>
-      <c r="N68" s="78"/>
-      <c r="O68" s="78"/>
-      <c r="P68" s="78"/>
-      <c r="Q68" s="78"/>
-      <c r="R68" s="78"/>
-      <c r="S68" s="78"/>
-      <c r="T68" s="78"/>
-      <c r="U68" s="78"/>
-      <c r="V68" s="78"/>
-      <c r="W68" s="78"/>
-      <c r="X68" s="78"/>
-      <c r="Y68" s="78"/>
+      <c r="C68" s="75"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="75"/>
+      <c r="F68" s="75"/>
+      <c r="G68" s="75"/>
+      <c r="H68" s="75"/>
+      <c r="I68" s="75"/>
+      <c r="J68" s="75"/>
+      <c r="K68" s="75"/>
+      <c r="L68" s="75"/>
+      <c r="M68" s="75"/>
+      <c r="N68" s="75"/>
+      <c r="O68" s="75"/>
+      <c r="P68" s="75"/>
+      <c r="Q68" s="75"/>
+      <c r="R68" s="75"/>
+      <c r="S68" s="75"/>
+      <c r="T68" s="75"/>
+      <c r="U68" s="75"/>
+      <c r="V68" s="75"/>
+      <c r="W68" s="75"/>
+      <c r="X68" s="75"/>
+      <c r="Y68" s="75"/>
     </row>
     <row r="70" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="77" t="s">
+      <c r="B70" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="77"/>
-      <c r="D70" s="77"/>
-      <c r="E70" s="77"/>
-      <c r="F70" s="77"/>
-      <c r="G70" s="77"/>
-      <c r="H70" s="77"/>
-      <c r="I70" s="77"/>
-      <c r="J70" s="77"/>
-      <c r="L70" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="M70" s="60"/>
-      <c r="N70" s="60"/>
-      <c r="O70" s="60"/>
-      <c r="P70" s="60"/>
-      <c r="Q70" s="60"/>
-      <c r="R70" s="60"/>
-      <c r="S70" s="60"/>
-      <c r="T70" s="60"/>
-      <c r="V70" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="W70" s="60"/>
-      <c r="X70" s="60"/>
-      <c r="Y70" s="60"/>
-      <c r="Z70" s="60"/>
-      <c r="AA70" s="60"/>
-      <c r="AB70" s="60"/>
-      <c r="AC70" s="60"/>
-      <c r="AD70" s="60"/>
+      <c r="C70" s="78"/>
+      <c r="D70" s="78"/>
+      <c r="E70" s="78"/>
+      <c r="F70" s="78"/>
+      <c r="G70" s="78"/>
+      <c r="H70" s="78"/>
+      <c r="I70" s="78"/>
+      <c r="J70" s="78"/>
+      <c r="L70" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="M70" s="79"/>
+      <c r="N70" s="79"/>
+      <c r="O70" s="79"/>
+      <c r="P70" s="79"/>
+      <c r="Q70" s="79"/>
+      <c r="R70" s="79"/>
+      <c r="S70" s="79"/>
+      <c r="T70" s="79"/>
+      <c r="V70" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="W70" s="79"/>
+      <c r="X70" s="79"/>
+      <c r="Y70" s="79"/>
+      <c r="Z70" s="79"/>
+      <c r="AA70" s="79"/>
+      <c r="AB70" s="79"/>
+      <c r="AC70" s="79"/>
+      <c r="AD70" s="79"/>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
@@ -6015,51 +6080,51 @@
     </row>
     <row r="72" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="15"/>
-      <c r="C72" s="61" t="s">
+      <c r="C72" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
-      <c r="H72" s="61"/>
-      <c r="I72" s="61"/>
-      <c r="J72" s="62"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="59"/>
       <c r="L72" s="15"/>
-      <c r="M72" s="61" t="s">
+      <c r="M72" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="N72" s="61"/>
-      <c r="O72" s="61"/>
-      <c r="P72" s="61"/>
-      <c r="Q72" s="61"/>
-      <c r="R72" s="61"/>
-      <c r="S72" s="61"/>
-      <c r="T72" s="62"/>
+      <c r="N72" s="58"/>
+      <c r="O72" s="58"/>
+      <c r="P72" s="58"/>
+      <c r="Q72" s="58"/>
+      <c r="R72" s="58"/>
+      <c r="S72" s="58"/>
+      <c r="T72" s="59"/>
       <c r="V72" s="15"/>
-      <c r="W72" s="61" t="s">
+      <c r="W72" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="X72" s="61"/>
-      <c r="Y72" s="61"/>
-      <c r="Z72" s="61"/>
-      <c r="AA72" s="61"/>
-      <c r="AB72" s="61"/>
-      <c r="AC72" s="61"/>
-      <c r="AD72" s="62"/>
+      <c r="X72" s="58"/>
+      <c r="Y72" s="58"/>
+      <c r="Z72" s="58"/>
+      <c r="AA72" s="58"/>
+      <c r="AB72" s="58"/>
+      <c r="AC72" s="58"/>
+      <c r="AD72" s="59"/>
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B73" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C73" s="63" t="s">
+      <c r="C73" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="64"/>
-      <c r="E73" s="65" t="s">
+      <c r="D73" s="61"/>
+      <c r="E73" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F73" s="65"/>
+      <c r="F73" s="56"/>
       <c r="G73" s="20" t="s">
         <v>23</v>
       </c>
@@ -6075,14 +6140,14 @@
       <c r="L73" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M73" s="63" t="s">
+      <c r="M73" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="N73" s="64"/>
-      <c r="O73" s="65" t="s">
+      <c r="N73" s="61"/>
+      <c r="O73" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="P73" s="65"/>
+      <c r="P73" s="56"/>
       <c r="Q73" s="20" t="s">
         <v>23</v>
       </c>
@@ -6098,14 +6163,14 @@
       <c r="V73" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="W73" s="63" t="s">
+      <c r="W73" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="X73" s="64"/>
-      <c r="Y73" s="65" t="s">
+      <c r="X73" s="61"/>
+      <c r="Y73" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="Z73" s="65"/>
+      <c r="Z73" s="56"/>
       <c r="AA73" s="20" t="s">
         <v>23</v>
       </c>
@@ -6145,7 +6210,7 @@
         <v>39</v>
       </c>
       <c r="J74" s="37" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="L74" s="12" t="s">
         <v>17</v>
@@ -6172,7 +6237,7 @@
         <v>41</v>
       </c>
       <c r="T74" s="37" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="V74" s="12" t="s">
         <v>17</v>
@@ -6199,32 +6264,32 @@
         <v>38</v>
       </c>
       <c r="AD74" s="37" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L76" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="M76" s="60"/>
-      <c r="N76" s="60"/>
-      <c r="O76" s="60"/>
-      <c r="P76" s="60"/>
-      <c r="Q76" s="60"/>
-      <c r="R76" s="60"/>
-      <c r="S76" s="60"/>
-      <c r="T76" s="60"/>
-      <c r="V76" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="W76" s="60"/>
-      <c r="X76" s="60"/>
-      <c r="Y76" s="60"/>
-      <c r="Z76" s="60"/>
-      <c r="AA76" s="60"/>
-      <c r="AB76" s="60"/>
-      <c r="AC76" s="60"/>
-      <c r="AD76" s="60"/>
+      <c r="L76" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="M76" s="79"/>
+      <c r="N76" s="79"/>
+      <c r="O76" s="79"/>
+      <c r="P76" s="79"/>
+      <c r="Q76" s="79"/>
+      <c r="R76" s="79"/>
+      <c r="S76" s="79"/>
+      <c r="T76" s="79"/>
+      <c r="V76" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="W76" s="79"/>
+      <c r="X76" s="79"/>
+      <c r="Y76" s="79"/>
+      <c r="Z76" s="79"/>
+      <c r="AA76" s="79"/>
+      <c r="AB76" s="79"/>
+      <c r="AC76" s="79"/>
+      <c r="AD76" s="79"/>
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L77" s="9" t="s">
@@ -6284,40 +6349,40 @@
     </row>
     <row r="78" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L78" s="15"/>
-      <c r="M78" s="61" t="s">
+      <c r="M78" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="N78" s="61"/>
-      <c r="O78" s="61"/>
-      <c r="P78" s="61"/>
-      <c r="Q78" s="61"/>
-      <c r="R78" s="61"/>
-      <c r="S78" s="61"/>
-      <c r="T78" s="62"/>
+      <c r="N78" s="58"/>
+      <c r="O78" s="58"/>
+      <c r="P78" s="58"/>
+      <c r="Q78" s="58"/>
+      <c r="R78" s="58"/>
+      <c r="S78" s="58"/>
+      <c r="T78" s="59"/>
       <c r="V78" s="15"/>
-      <c r="W78" s="61" t="s">
+      <c r="W78" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="X78" s="61"/>
-      <c r="Y78" s="61"/>
-      <c r="Z78" s="61"/>
-      <c r="AA78" s="61"/>
-      <c r="AB78" s="61"/>
-      <c r="AC78" s="61"/>
-      <c r="AD78" s="62"/>
+      <c r="X78" s="58"/>
+      <c r="Y78" s="58"/>
+      <c r="Z78" s="58"/>
+      <c r="AA78" s="58"/>
+      <c r="AB78" s="58"/>
+      <c r="AC78" s="58"/>
+      <c r="AD78" s="59"/>
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L79" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M79" s="63" t="s">
+      <c r="M79" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="N79" s="64"/>
-      <c r="O79" s="65" t="s">
+      <c r="N79" s="61"/>
+      <c r="O79" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="P79" s="65"/>
+      <c r="P79" s="56"/>
       <c r="Q79" s="20" t="s">
         <v>23</v>
       </c>
@@ -6333,14 +6398,14 @@
       <c r="V79" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="W79" s="63" t="s">
+      <c r="W79" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="X79" s="64"/>
-      <c r="Y79" s="65" t="s">
+      <c r="X79" s="61"/>
+      <c r="Y79" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="Z79" s="65"/>
+      <c r="Z79" s="56"/>
       <c r="AA79" s="20" t="s">
         <v>23</v>
       </c>
@@ -6380,7 +6445,7 @@
         <v>44</v>
       </c>
       <c r="T80" s="37" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="V80" s="12" t="s">
         <v>17</v>
@@ -6407,15 +6472,15 @@
         <v>46</v>
       </c>
       <c r="AD80" s="37" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B83" s="66" t="s">
+      <c r="B83" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="67"/>
+      <c r="C83" s="77"/>
       <c r="D83" s="68" t="s">
         <v>4</v>
       </c>
@@ -6441,7 +6506,7 @@
       </c>
       <c r="C84" s="71"/>
       <c r="D84" s="72" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E84" s="73"/>
       <c r="F84" s="73"/>
@@ -6460,57 +6525,57 @@
       <c r="S84" s="74"/>
     </row>
     <row r="85" spans="1:25" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="56" t="s">
+      <c r="B85" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C85" s="57"/>
-      <c r="D85" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="E85" s="58"/>
-      <c r="F85" s="58"/>
-      <c r="G85" s="58"/>
-      <c r="H85" s="58"/>
-      <c r="I85" s="58"/>
-      <c r="J85" s="58"/>
-      <c r="K85" s="58"/>
-      <c r="L85" s="58"/>
-      <c r="M85" s="58"/>
-      <c r="N85" s="58"/>
-      <c r="O85" s="58"/>
-      <c r="P85" s="58"/>
-      <c r="Q85" s="58"/>
-      <c r="R85" s="58"/>
-      <c r="S85" s="59"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E85" s="66"/>
+      <c r="F85" s="66"/>
+      <c r="G85" s="66"/>
+      <c r="H85" s="66"/>
+      <c r="I85" s="66"/>
+      <c r="J85" s="66"/>
+      <c r="K85" s="66"/>
+      <c r="L85" s="66"/>
+      <c r="M85" s="66"/>
+      <c r="N85" s="66"/>
+      <c r="O85" s="66"/>
+      <c r="P85" s="66"/>
+      <c r="Q85" s="66"/>
+      <c r="R85" s="66"/>
+      <c r="S85" s="67"/>
     </row>
     <row r="88" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A88" s="30"/>
-      <c r="B88" s="78" t="s">
+      <c r="B88" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="C88" s="78"/>
-      <c r="D88" s="78"/>
-      <c r="E88" s="78"/>
-      <c r="F88" s="78"/>
-      <c r="G88" s="78"/>
-      <c r="H88" s="78"/>
-      <c r="I88" s="78"/>
-      <c r="J88" s="78"/>
-      <c r="K88" s="78"/>
-      <c r="L88" s="78"/>
-      <c r="M88" s="78"/>
-      <c r="N88" s="78"/>
-      <c r="O88" s="78"/>
-      <c r="P88" s="78"/>
-      <c r="Q88" s="78"/>
-      <c r="R88" s="78"/>
-      <c r="S88" s="78"/>
-      <c r="T88" s="78"/>
-      <c r="U88" s="78"/>
-      <c r="V88" s="78"/>
-      <c r="W88" s="78"/>
-      <c r="X88" s="78"/>
-      <c r="Y88" s="78"/>
+      <c r="C88" s="75"/>
+      <c r="D88" s="75"/>
+      <c r="E88" s="75"/>
+      <c r="F88" s="75"/>
+      <c r="G88" s="75"/>
+      <c r="H88" s="75"/>
+      <c r="I88" s="75"/>
+      <c r="J88" s="75"/>
+      <c r="K88" s="75"/>
+      <c r="L88" s="75"/>
+      <c r="M88" s="75"/>
+      <c r="N88" s="75"/>
+      <c r="O88" s="75"/>
+      <c r="P88" s="75"/>
+      <c r="Q88" s="75"/>
+      <c r="R88" s="75"/>
+      <c r="S88" s="75"/>
+      <c r="T88" s="75"/>
+      <c r="U88" s="75"/>
+      <c r="V88" s="75"/>
+      <c r="W88" s="75"/>
+      <c r="X88" s="75"/>
+      <c r="Y88" s="75"/>
     </row>
     <row r="89" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
@@ -6556,35 +6621,35 @@
     </row>
     <row r="91" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B91" s="15"/>
-      <c r="C91" s="61" t="s">
+      <c r="C91" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D91" s="61"/>
-      <c r="E91" s="61"/>
-      <c r="F91" s="61"/>
-      <c r="G91" s="61"/>
-      <c r="H91" s="61"/>
-      <c r="I91" s="61"/>
-      <c r="J91" s="62"/>
-      <c r="K91" s="79" t="s">
+      <c r="D91" s="58"/>
+      <c r="E91" s="58"/>
+      <c r="F91" s="58"/>
+      <c r="G91" s="58"/>
+      <c r="H91" s="58"/>
+      <c r="I91" s="58"/>
+      <c r="J91" s="59"/>
+      <c r="K91" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="L91" s="80"/>
-      <c r="M91" s="80"/>
-      <c r="N91" s="81"/>
+      <c r="L91" s="84"/>
+      <c r="M91" s="84"/>
+      <c r="N91" s="85"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B92" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C92" s="63" t="s">
+      <c r="C92" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="64"/>
-      <c r="E92" s="65" t="s">
+      <c r="D92" s="61"/>
+      <c r="E92" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F92" s="65"/>
+      <c r="F92" s="56"/>
       <c r="G92" s="20" t="s">
         <v>23</v>
       </c>
@@ -6597,12 +6662,12 @@
       <c r="J92" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="K92" s="107" t="s">
+      <c r="K92" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="L92" s="108"/>
-      <c r="M92" s="108"/>
-      <c r="N92" s="109"/>
+      <c r="L92" s="113"/>
+      <c r="M92" s="113"/>
+      <c r="N92" s="114"/>
     </row>
     <row r="93" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="12" t="s">
@@ -6647,10 +6712,10 @@
     </row>
     <row r="94" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B95" s="66" t="s">
+      <c r="B95" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="67"/>
+      <c r="C95" s="77"/>
       <c r="D95" s="68" t="s">
         <v>4</v>
       </c>
@@ -6676,7 +6741,7 @@
       </c>
       <c r="C96" s="71"/>
       <c r="D96" s="72" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E96" s="73"/>
       <c r="F96" s="73"/>
@@ -6695,12 +6760,12 @@
       <c r="S96" s="74"/>
     </row>
     <row r="97" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="75" t="s">
+      <c r="B97" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="C97" s="76"/>
+      <c r="C97" s="116"/>
       <c r="D97" s="72" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E97" s="73"/>
       <c r="F97" s="73"/>
@@ -6720,10 +6785,10 @@
     </row>
     <row r="98" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B99" s="66" t="s">
+      <c r="B99" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C99" s="67"/>
+      <c r="C99" s="77"/>
       <c r="D99" s="68" t="s">
         <v>4</v>
       </c>
@@ -6768,92 +6833,92 @@
       <c r="S100" s="74"/>
     </row>
     <row r="101" spans="1:30" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="56" t="s">
+      <c r="B101" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C101" s="57"/>
-      <c r="D101" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="E101" s="58"/>
-      <c r="F101" s="58"/>
-      <c r="G101" s="58"/>
-      <c r="H101" s="58"/>
-      <c r="I101" s="58"/>
-      <c r="J101" s="58"/>
-      <c r="K101" s="58"/>
-      <c r="L101" s="58"/>
-      <c r="M101" s="58"/>
-      <c r="N101" s="58"/>
-      <c r="O101" s="58"/>
-      <c r="P101" s="58"/>
-      <c r="Q101" s="58"/>
-      <c r="R101" s="58"/>
-      <c r="S101" s="59"/>
+      <c r="C101" s="65"/>
+      <c r="D101" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E101" s="66"/>
+      <c r="F101" s="66"/>
+      <c r="G101" s="66"/>
+      <c r="H101" s="66"/>
+      <c r="I101" s="66"/>
+      <c r="J101" s="66"/>
+      <c r="K101" s="66"/>
+      <c r="L101" s="66"/>
+      <c r="M101" s="66"/>
+      <c r="N101" s="66"/>
+      <c r="O101" s="66"/>
+      <c r="P101" s="66"/>
+      <c r="Q101" s="66"/>
+      <c r="R101" s="66"/>
+      <c r="S101" s="67"/>
     </row>
     <row r="104" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A104" s="30"/>
-      <c r="B104" s="78" t="s">
+      <c r="B104" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="C104" s="78"/>
-      <c r="D104" s="78"/>
-      <c r="E104" s="78"/>
-      <c r="F104" s="78"/>
-      <c r="G104" s="78"/>
-      <c r="H104" s="78"/>
-      <c r="I104" s="78"/>
-      <c r="J104" s="78"/>
-      <c r="K104" s="78"/>
-      <c r="L104" s="78"/>
-      <c r="M104" s="78"/>
-      <c r="N104" s="78"/>
-      <c r="O104" s="78"/>
-      <c r="P104" s="78"/>
-      <c r="Q104" s="78"/>
-      <c r="R104" s="78"/>
-      <c r="S104" s="78"/>
-      <c r="T104" s="78"/>
-      <c r="U104" s="78"/>
-      <c r="V104" s="78"/>
-      <c r="W104" s="78"/>
-      <c r="X104" s="78"/>
-      <c r="Y104" s="78"/>
+      <c r="C104" s="75"/>
+      <c r="D104" s="75"/>
+      <c r="E104" s="75"/>
+      <c r="F104" s="75"/>
+      <c r="G104" s="75"/>
+      <c r="H104" s="75"/>
+      <c r="I104" s="75"/>
+      <c r="J104" s="75"/>
+      <c r="K104" s="75"/>
+      <c r="L104" s="75"/>
+      <c r="M104" s="75"/>
+      <c r="N104" s="75"/>
+      <c r="O104" s="75"/>
+      <c r="P104" s="75"/>
+      <c r="Q104" s="75"/>
+      <c r="R104" s="75"/>
+      <c r="S104" s="75"/>
+      <c r="T104" s="75"/>
+      <c r="U104" s="75"/>
+      <c r="V104" s="75"/>
+      <c r="W104" s="75"/>
+      <c r="X104" s="75"/>
+      <c r="Y104" s="75"/>
     </row>
     <row r="106" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="77" t="s">
+      <c r="B106" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C106" s="77"/>
-      <c r="D106" s="77"/>
-      <c r="E106" s="77"/>
-      <c r="F106" s="77"/>
-      <c r="G106" s="77"/>
-      <c r="H106" s="77"/>
-      <c r="I106" s="77"/>
-      <c r="J106" s="77"/>
-      <c r="L106" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="M106" s="60"/>
-      <c r="N106" s="60"/>
-      <c r="O106" s="60"/>
-      <c r="P106" s="60"/>
-      <c r="Q106" s="60"/>
-      <c r="R106" s="60"/>
-      <c r="S106" s="60"/>
-      <c r="T106" s="60"/>
-      <c r="V106" s="60" t="s">
+      <c r="C106" s="78"/>
+      <c r="D106" s="78"/>
+      <c r="E106" s="78"/>
+      <c r="F106" s="78"/>
+      <c r="G106" s="78"/>
+      <c r="H106" s="78"/>
+      <c r="I106" s="78"/>
+      <c r="J106" s="78"/>
+      <c r="L106" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="M106" s="79"/>
+      <c r="N106" s="79"/>
+      <c r="O106" s="79"/>
+      <c r="P106" s="79"/>
+      <c r="Q106" s="79"/>
+      <c r="R106" s="79"/>
+      <c r="S106" s="79"/>
+      <c r="T106" s="79"/>
+      <c r="V106" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="W106" s="60"/>
-      <c r="X106" s="60"/>
-      <c r="Y106" s="60"/>
-      <c r="Z106" s="60"/>
-      <c r="AA106" s="60"/>
-      <c r="AB106" s="60"/>
-      <c r="AC106" s="60"/>
-      <c r="AD106" s="60"/>
+      <c r="W106" s="79"/>
+      <c r="X106" s="79"/>
+      <c r="Y106" s="79"/>
+      <c r="Z106" s="79"/>
+      <c r="AA106" s="79"/>
+      <c r="AB106" s="79"/>
+      <c r="AC106" s="79"/>
+      <c r="AD106" s="79"/>
     </row>
     <row r="107" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B107" s="9" t="s">
@@ -6940,51 +7005,51 @@
     </row>
     <row r="108" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B108" s="15"/>
-      <c r="C108" s="61" t="s">
+      <c r="C108" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D108" s="61"/>
-      <c r="E108" s="61"/>
-      <c r="F108" s="61"/>
-      <c r="G108" s="61"/>
-      <c r="H108" s="61"/>
-      <c r="I108" s="61"/>
-      <c r="J108" s="62"/>
+      <c r="D108" s="58"/>
+      <c r="E108" s="58"/>
+      <c r="F108" s="58"/>
+      <c r="G108" s="58"/>
+      <c r="H108" s="58"/>
+      <c r="I108" s="58"/>
+      <c r="J108" s="59"/>
       <c r="L108" s="15"/>
-      <c r="M108" s="61" t="s">
+      <c r="M108" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="N108" s="61"/>
-      <c r="O108" s="61"/>
-      <c r="P108" s="61"/>
-      <c r="Q108" s="61"/>
-      <c r="R108" s="61"/>
-      <c r="S108" s="61"/>
-      <c r="T108" s="62"/>
+      <c r="N108" s="58"/>
+      <c r="O108" s="58"/>
+      <c r="P108" s="58"/>
+      <c r="Q108" s="58"/>
+      <c r="R108" s="58"/>
+      <c r="S108" s="58"/>
+      <c r="T108" s="59"/>
       <c r="V108" s="15"/>
-      <c r="W108" s="61" t="s">
+      <c r="W108" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="X108" s="61"/>
-      <c r="Y108" s="61"/>
-      <c r="Z108" s="61"/>
-      <c r="AA108" s="61"/>
-      <c r="AB108" s="61"/>
-      <c r="AC108" s="61"/>
-      <c r="AD108" s="62"/>
+      <c r="X108" s="58"/>
+      <c r="Y108" s="58"/>
+      <c r="Z108" s="58"/>
+      <c r="AA108" s="58"/>
+      <c r="AB108" s="58"/>
+      <c r="AC108" s="58"/>
+      <c r="AD108" s="59"/>
     </row>
     <row r="109" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B109" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C109" s="63" t="s">
+      <c r="C109" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D109" s="64"/>
-      <c r="E109" s="65" t="s">
+      <c r="D109" s="61"/>
+      <c r="E109" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F109" s="65"/>
+      <c r="F109" s="56"/>
       <c r="G109" s="20" t="s">
         <v>23</v>
       </c>
@@ -7000,14 +7065,14 @@
       <c r="L109" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M109" s="63" t="s">
+      <c r="M109" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="N109" s="64"/>
-      <c r="O109" s="65" t="s">
+      <c r="N109" s="61"/>
+      <c r="O109" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="P109" s="65"/>
+      <c r="P109" s="56"/>
       <c r="Q109" s="20" t="s">
         <v>23</v>
       </c>
@@ -7023,14 +7088,14 @@
       <c r="V109" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="W109" s="63" t="s">
+      <c r="W109" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="X109" s="64"/>
-      <c r="Y109" s="65" t="s">
+      <c r="X109" s="61"/>
+      <c r="Y109" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="Z109" s="65"/>
+      <c r="Z109" s="56"/>
       <c r="AA109" s="20" t="s">
         <v>23</v>
       </c>
@@ -7070,7 +7135,7 @@
         <v>39</v>
       </c>
       <c r="J110" s="37" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="L110" s="12" t="s">
         <v>17</v>
@@ -7097,7 +7162,7 @@
         <v>41</v>
       </c>
       <c r="T110" s="37" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="V110" s="12" t="s">
         <v>17</v>
@@ -7124,15 +7189,15 @@
         <v>63</v>
       </c>
       <c r="AD110" s="37" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="112" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B112" s="66" t="s">
+      <c r="B112" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C112" s="67"/>
+      <c r="C112" s="77"/>
       <c r="D112" s="68" t="s">
         <v>4</v>
       </c>
@@ -7158,7 +7223,7 @@
       </c>
       <c r="C113" s="71"/>
       <c r="D113" s="72" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E113" s="73"/>
       <c r="F113" s="73"/>
@@ -7177,57 +7242,57 @@
       <c r="S113" s="74"/>
     </row>
     <row r="114" spans="1:25" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="56" t="s">
+      <c r="B114" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C114" s="57"/>
-      <c r="D114" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="E114" s="58"/>
-      <c r="F114" s="58"/>
-      <c r="G114" s="58"/>
-      <c r="H114" s="58"/>
-      <c r="I114" s="58"/>
-      <c r="J114" s="58"/>
-      <c r="K114" s="58"/>
-      <c r="L114" s="58"/>
-      <c r="M114" s="58"/>
-      <c r="N114" s="58"/>
-      <c r="O114" s="58"/>
-      <c r="P114" s="58"/>
-      <c r="Q114" s="58"/>
-      <c r="R114" s="58"/>
-      <c r="S114" s="59"/>
+      <c r="C114" s="65"/>
+      <c r="D114" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E114" s="66"/>
+      <c r="F114" s="66"/>
+      <c r="G114" s="66"/>
+      <c r="H114" s="66"/>
+      <c r="I114" s="66"/>
+      <c r="J114" s="66"/>
+      <c r="K114" s="66"/>
+      <c r="L114" s="66"/>
+      <c r="M114" s="66"/>
+      <c r="N114" s="66"/>
+      <c r="O114" s="66"/>
+      <c r="P114" s="66"/>
+      <c r="Q114" s="66"/>
+      <c r="R114" s="66"/>
+      <c r="S114" s="67"/>
     </row>
     <row r="117" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A117" s="30"/>
-      <c r="B117" s="78" t="s">
+      <c r="B117" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="C117" s="78"/>
-      <c r="D117" s="78"/>
-      <c r="E117" s="78"/>
-      <c r="F117" s="78"/>
-      <c r="G117" s="78"/>
-      <c r="H117" s="78"/>
-      <c r="I117" s="78"/>
-      <c r="J117" s="78"/>
-      <c r="K117" s="78"/>
-      <c r="L117" s="78"/>
-      <c r="M117" s="78"/>
-      <c r="N117" s="78"/>
-      <c r="O117" s="78"/>
-      <c r="P117" s="78"/>
-      <c r="Q117" s="78"/>
-      <c r="R117" s="78"/>
-      <c r="S117" s="78"/>
-      <c r="T117" s="78"/>
-      <c r="U117" s="78"/>
-      <c r="V117" s="78"/>
-      <c r="W117" s="78"/>
-      <c r="X117" s="78"/>
-      <c r="Y117" s="78"/>
+      <c r="C117" s="75"/>
+      <c r="D117" s="75"/>
+      <c r="E117" s="75"/>
+      <c r="F117" s="75"/>
+      <c r="G117" s="75"/>
+      <c r="H117" s="75"/>
+      <c r="I117" s="75"/>
+      <c r="J117" s="75"/>
+      <c r="K117" s="75"/>
+      <c r="L117" s="75"/>
+      <c r="M117" s="75"/>
+      <c r="N117" s="75"/>
+      <c r="O117" s="75"/>
+      <c r="P117" s="75"/>
+      <c r="Q117" s="75"/>
+      <c r="R117" s="75"/>
+      <c r="S117" s="75"/>
+      <c r="T117" s="75"/>
+      <c r="U117" s="75"/>
+      <c r="V117" s="75"/>
+      <c r="W117" s="75"/>
+      <c r="X117" s="75"/>
+      <c r="Y117" s="75"/>
     </row>
     <row r="118" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="119" spans="1:25" x14ac:dyDescent="0.25">
@@ -7261,29 +7326,29 @@
     </row>
     <row r="120" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B120" s="15"/>
-      <c r="C120" s="61" t="s">
+      <c r="C120" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D120" s="61"/>
-      <c r="E120" s="61"/>
-      <c r="F120" s="61"/>
-      <c r="G120" s="61"/>
-      <c r="H120" s="61"/>
-      <c r="I120" s="61"/>
-      <c r="J120" s="62"/>
+      <c r="D120" s="58"/>
+      <c r="E120" s="58"/>
+      <c r="F120" s="58"/>
+      <c r="G120" s="58"/>
+      <c r="H120" s="58"/>
+      <c r="I120" s="58"/>
+      <c r="J120" s="59"/>
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B121" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C121" s="63" t="s">
+      <c r="C121" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D121" s="64"/>
-      <c r="E121" s="65" t="s">
+      <c r="D121" s="61"/>
+      <c r="E121" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F121" s="65"/>
+      <c r="F121" s="56"/>
       <c r="G121" s="20" t="s">
         <v>23</v>
       </c>
@@ -7323,15 +7388,15 @@
         <v>39</v>
       </c>
       <c r="J122" s="37" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="124" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B124" s="66" t="s">
+      <c r="B124" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C124" s="67"/>
+      <c r="C124" s="77"/>
       <c r="D124" s="68" t="s">
         <v>4</v>
       </c>
@@ -7357,7 +7422,7 @@
       </c>
       <c r="C125" s="71"/>
       <c r="D125" s="72" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E125" s="73"/>
       <c r="F125" s="73"/>
@@ -7376,92 +7441,92 @@
       <c r="S125" s="74"/>
     </row>
     <row r="126" spans="1:25" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="56" t="s">
+      <c r="B126" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C126" s="57"/>
-      <c r="D126" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="E126" s="58"/>
-      <c r="F126" s="58"/>
-      <c r="G126" s="58"/>
-      <c r="H126" s="58"/>
-      <c r="I126" s="58"/>
-      <c r="J126" s="58"/>
-      <c r="K126" s="58"/>
-      <c r="L126" s="58"/>
-      <c r="M126" s="58"/>
-      <c r="N126" s="58"/>
-      <c r="O126" s="58"/>
-      <c r="P126" s="58"/>
-      <c r="Q126" s="58"/>
-      <c r="R126" s="58"/>
-      <c r="S126" s="59"/>
+      <c r="C126" s="65"/>
+      <c r="D126" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E126" s="66"/>
+      <c r="F126" s="66"/>
+      <c r="G126" s="66"/>
+      <c r="H126" s="66"/>
+      <c r="I126" s="66"/>
+      <c r="J126" s="66"/>
+      <c r="K126" s="66"/>
+      <c r="L126" s="66"/>
+      <c r="M126" s="66"/>
+      <c r="N126" s="66"/>
+      <c r="O126" s="66"/>
+      <c r="P126" s="66"/>
+      <c r="Q126" s="66"/>
+      <c r="R126" s="66"/>
+      <c r="S126" s="67"/>
     </row>
     <row r="129" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A129" s="30"/>
-      <c r="B129" s="78" t="s">
+      <c r="B129" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="C129" s="78"/>
-      <c r="D129" s="78"/>
-      <c r="E129" s="78"/>
-      <c r="F129" s="78"/>
-      <c r="G129" s="78"/>
-      <c r="H129" s="78"/>
-      <c r="I129" s="78"/>
-      <c r="J129" s="78"/>
-      <c r="K129" s="78"/>
-      <c r="L129" s="78"/>
-      <c r="M129" s="78"/>
-      <c r="N129" s="78"/>
-      <c r="O129" s="78"/>
-      <c r="P129" s="78"/>
-      <c r="Q129" s="78"/>
-      <c r="R129" s="78"/>
-      <c r="S129" s="78"/>
-      <c r="T129" s="78"/>
-      <c r="U129" s="78"/>
-      <c r="V129" s="78"/>
-      <c r="W129" s="78"/>
-      <c r="X129" s="78"/>
-      <c r="Y129" s="78"/>
+      <c r="C129" s="75"/>
+      <c r="D129" s="75"/>
+      <c r="E129" s="75"/>
+      <c r="F129" s="75"/>
+      <c r="G129" s="75"/>
+      <c r="H129" s="75"/>
+      <c r="I129" s="75"/>
+      <c r="J129" s="75"/>
+      <c r="K129" s="75"/>
+      <c r="L129" s="75"/>
+      <c r="M129" s="75"/>
+      <c r="N129" s="75"/>
+      <c r="O129" s="75"/>
+      <c r="P129" s="75"/>
+      <c r="Q129" s="75"/>
+      <c r="R129" s="75"/>
+      <c r="S129" s="75"/>
+      <c r="T129" s="75"/>
+      <c r="U129" s="75"/>
+      <c r="V129" s="75"/>
+      <c r="W129" s="75"/>
+      <c r="X129" s="75"/>
+      <c r="Y129" s="75"/>
     </row>
     <row r="131" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="77" t="s">
+      <c r="B131" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C131" s="77"/>
-      <c r="D131" s="77"/>
-      <c r="E131" s="77"/>
-      <c r="F131" s="77"/>
-      <c r="G131" s="77"/>
-      <c r="H131" s="77"/>
-      <c r="I131" s="77"/>
-      <c r="J131" s="77"/>
-      <c r="L131" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="M131" s="60"/>
-      <c r="N131" s="60"/>
-      <c r="O131" s="60"/>
-      <c r="P131" s="60"/>
-      <c r="Q131" s="60"/>
-      <c r="R131" s="60"/>
-      <c r="S131" s="60"/>
-      <c r="T131" s="60"/>
-      <c r="V131" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="W131" s="60"/>
-      <c r="X131" s="60"/>
-      <c r="Y131" s="60"/>
-      <c r="Z131" s="60"/>
-      <c r="AA131" s="60"/>
-      <c r="AB131" s="60"/>
-      <c r="AC131" s="60"/>
-      <c r="AD131" s="60"/>
+      <c r="C131" s="78"/>
+      <c r="D131" s="78"/>
+      <c r="E131" s="78"/>
+      <c r="F131" s="78"/>
+      <c r="G131" s="78"/>
+      <c r="H131" s="78"/>
+      <c r="I131" s="78"/>
+      <c r="J131" s="78"/>
+      <c r="L131" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="M131" s="79"/>
+      <c r="N131" s="79"/>
+      <c r="O131" s="79"/>
+      <c r="P131" s="79"/>
+      <c r="Q131" s="79"/>
+      <c r="R131" s="79"/>
+      <c r="S131" s="79"/>
+      <c r="T131" s="79"/>
+      <c r="V131" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="W131" s="79"/>
+      <c r="X131" s="79"/>
+      <c r="Y131" s="79"/>
+      <c r="Z131" s="79"/>
+      <c r="AA131" s="79"/>
+      <c r="AB131" s="79"/>
+      <c r="AC131" s="79"/>
+      <c r="AD131" s="79"/>
     </row>
     <row r="132" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B132" s="9" t="s">
@@ -7548,51 +7613,51 @@
     </row>
     <row r="133" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B133" s="15"/>
-      <c r="C133" s="61" t="s">
+      <c r="C133" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D133" s="61"/>
-      <c r="E133" s="61"/>
-      <c r="F133" s="61"/>
-      <c r="G133" s="61"/>
-      <c r="H133" s="61"/>
-      <c r="I133" s="61"/>
-      <c r="J133" s="62"/>
+      <c r="D133" s="58"/>
+      <c r="E133" s="58"/>
+      <c r="F133" s="58"/>
+      <c r="G133" s="58"/>
+      <c r="H133" s="58"/>
+      <c r="I133" s="58"/>
+      <c r="J133" s="59"/>
       <c r="L133" s="15"/>
-      <c r="M133" s="61" t="s">
+      <c r="M133" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="N133" s="61"/>
-      <c r="O133" s="61"/>
-      <c r="P133" s="61"/>
-      <c r="Q133" s="61"/>
-      <c r="R133" s="61"/>
-      <c r="S133" s="61"/>
-      <c r="T133" s="62"/>
+      <c r="N133" s="58"/>
+      <c r="O133" s="58"/>
+      <c r="P133" s="58"/>
+      <c r="Q133" s="58"/>
+      <c r="R133" s="58"/>
+      <c r="S133" s="58"/>
+      <c r="T133" s="59"/>
       <c r="V133" s="15"/>
-      <c r="W133" s="61" t="s">
+      <c r="W133" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="X133" s="61"/>
-      <c r="Y133" s="61"/>
-      <c r="Z133" s="61"/>
-      <c r="AA133" s="61"/>
-      <c r="AB133" s="61"/>
-      <c r="AC133" s="61"/>
-      <c r="AD133" s="62"/>
+      <c r="X133" s="58"/>
+      <c r="Y133" s="58"/>
+      <c r="Z133" s="58"/>
+      <c r="AA133" s="58"/>
+      <c r="AB133" s="58"/>
+      <c r="AC133" s="58"/>
+      <c r="AD133" s="59"/>
     </row>
     <row r="134" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B134" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C134" s="63" t="s">
+      <c r="C134" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D134" s="64"/>
-      <c r="E134" s="65" t="s">
+      <c r="D134" s="61"/>
+      <c r="E134" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F134" s="65"/>
+      <c r="F134" s="56"/>
       <c r="G134" s="20" t="s">
         <v>23</v>
       </c>
@@ -7608,14 +7673,14 @@
       <c r="L134" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M134" s="63" t="s">
+      <c r="M134" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="N134" s="64"/>
-      <c r="O134" s="65" t="s">
+      <c r="N134" s="61"/>
+      <c r="O134" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="P134" s="65"/>
+      <c r="P134" s="56"/>
       <c r="Q134" s="20" t="s">
         <v>23</v>
       </c>
@@ -7631,14 +7696,14 @@
       <c r="V134" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="W134" s="63" t="s">
+      <c r="W134" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="X134" s="64"/>
-      <c r="Y134" s="65" t="s">
+      <c r="X134" s="61"/>
+      <c r="Y134" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="Z134" s="65"/>
+      <c r="Z134" s="56"/>
       <c r="AA134" s="20" t="s">
         <v>23</v>
       </c>
@@ -7678,7 +7743,7 @@
         <v>39</v>
       </c>
       <c r="J135" s="37" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="L135" s="12" t="s">
         <v>17</v>
@@ -7705,7 +7770,7 @@
         <v>41</v>
       </c>
       <c r="T135" s="37" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="V135" s="12" t="s">
         <v>17</v>
@@ -7729,18 +7794,18 @@
         <v>65</v>
       </c>
       <c r="AC135" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="AD135" s="37" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
     </row>
     <row r="136" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="137" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B137" s="66" t="s">
+      <c r="B137" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C137" s="67"/>
+      <c r="C137" s="77"/>
       <c r="D137" s="68" t="s">
         <v>4</v>
       </c>
@@ -7766,7 +7831,7 @@
       </c>
       <c r="C138" s="71"/>
       <c r="D138" s="72" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E138" s="73"/>
       <c r="F138" s="73"/>
@@ -7785,57 +7850,57 @@
       <c r="S138" s="74"/>
     </row>
     <row r="139" spans="1:30" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="56" t="s">
+      <c r="B139" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C139" s="57"/>
-      <c r="D139" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="E139" s="58"/>
-      <c r="F139" s="58"/>
-      <c r="G139" s="58"/>
-      <c r="H139" s="58"/>
-      <c r="I139" s="58"/>
-      <c r="J139" s="58"/>
-      <c r="K139" s="58"/>
-      <c r="L139" s="58"/>
-      <c r="M139" s="58"/>
-      <c r="N139" s="58"/>
-      <c r="O139" s="58"/>
-      <c r="P139" s="58"/>
-      <c r="Q139" s="58"/>
-      <c r="R139" s="58"/>
-      <c r="S139" s="59"/>
+      <c r="C139" s="65"/>
+      <c r="D139" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="E139" s="66"/>
+      <c r="F139" s="66"/>
+      <c r="G139" s="66"/>
+      <c r="H139" s="66"/>
+      <c r="I139" s="66"/>
+      <c r="J139" s="66"/>
+      <c r="K139" s="66"/>
+      <c r="L139" s="66"/>
+      <c r="M139" s="66"/>
+      <c r="N139" s="66"/>
+      <c r="O139" s="66"/>
+      <c r="P139" s="66"/>
+      <c r="Q139" s="66"/>
+      <c r="R139" s="66"/>
+      <c r="S139" s="67"/>
     </row>
     <row r="142" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A142" s="30"/>
-      <c r="B142" s="78" t="s">
-        <v>123</v>
-      </c>
-      <c r="C142" s="78"/>
-      <c r="D142" s="78"/>
-      <c r="E142" s="78"/>
-      <c r="F142" s="78"/>
-      <c r="G142" s="78"/>
-      <c r="H142" s="78"/>
-      <c r="I142" s="78"/>
-      <c r="J142" s="78"/>
-      <c r="K142" s="78"/>
-      <c r="L142" s="78"/>
-      <c r="M142" s="78"/>
-      <c r="N142" s="78"/>
-      <c r="O142" s="78"/>
-      <c r="P142" s="78"/>
-      <c r="Q142" s="78"/>
-      <c r="R142" s="78"/>
-      <c r="S142" s="78"/>
-      <c r="T142" s="78"/>
-      <c r="U142" s="78"/>
-      <c r="V142" s="78"/>
-      <c r="W142" s="78"/>
-      <c r="X142" s="78"/>
-      <c r="Y142" s="78"/>
+      <c r="B142" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C142" s="75"/>
+      <c r="D142" s="75"/>
+      <c r="E142" s="75"/>
+      <c r="F142" s="75"/>
+      <c r="G142" s="75"/>
+      <c r="H142" s="75"/>
+      <c r="I142" s="75"/>
+      <c r="J142" s="75"/>
+      <c r="K142" s="75"/>
+      <c r="L142" s="75"/>
+      <c r="M142" s="75"/>
+      <c r="N142" s="75"/>
+      <c r="O142" s="75"/>
+      <c r="P142" s="75"/>
+      <c r="Q142" s="75"/>
+      <c r="R142" s="75"/>
+      <c r="S142" s="75"/>
+      <c r="T142" s="75"/>
+      <c r="U142" s="75"/>
+      <c r="V142" s="75"/>
+      <c r="W142" s="75"/>
+      <c r="X142" s="75"/>
+      <c r="Y142" s="75"/>
     </row>
     <row r="143" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="144" spans="1:30" x14ac:dyDescent="0.25">
@@ -7869,29 +7934,29 @@
     </row>
     <row r="145" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="15"/>
-      <c r="C145" s="61" t="s">
+      <c r="C145" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D145" s="61"/>
-      <c r="E145" s="61"/>
-      <c r="F145" s="61"/>
-      <c r="G145" s="61"/>
-      <c r="H145" s="61"/>
-      <c r="I145" s="61"/>
-      <c r="J145" s="62"/>
+      <c r="D145" s="58"/>
+      <c r="E145" s="58"/>
+      <c r="F145" s="58"/>
+      <c r="G145" s="58"/>
+      <c r="H145" s="58"/>
+      <c r="I145" s="58"/>
+      <c r="J145" s="59"/>
     </row>
     <row r="146" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B146" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C146" s="63" t="s">
+      <c r="C146" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D146" s="64"/>
-      <c r="E146" s="65" t="s">
+      <c r="D146" s="61"/>
+      <c r="E146" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F146" s="65"/>
+      <c r="F146" s="56"/>
       <c r="G146" s="20" t="s">
         <v>23</v>
       </c>
@@ -7925,21 +7990,21 @@
         <v>37</v>
       </c>
       <c r="H147" s="24" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="I147" s="19" t="s">
         <v>39</v>
       </c>
       <c r="J147" s="37" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="148" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="149" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B149" s="66" t="s">
+      <c r="B149" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C149" s="67"/>
+      <c r="C149" s="77"/>
       <c r="D149" s="68" t="s">
         <v>4</v>
       </c>
@@ -7965,7 +8030,7 @@
       </c>
       <c r="C150" s="71"/>
       <c r="D150" s="72" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E150" s="73"/>
       <c r="F150" s="73"/>
@@ -7984,85 +8049,85 @@
       <c r="S150" s="74"/>
     </row>
     <row r="151" spans="1:25" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="56" t="s">
+      <c r="B151" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C151" s="57"/>
-      <c r="D151" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="E151" s="58"/>
-      <c r="F151" s="58"/>
-      <c r="G151" s="58"/>
-      <c r="H151" s="58"/>
-      <c r="I151" s="58"/>
-      <c r="J151" s="58"/>
-      <c r="K151" s="58"/>
-      <c r="L151" s="58"/>
-      <c r="M151" s="58"/>
-      <c r="N151" s="58"/>
-      <c r="O151" s="58"/>
-      <c r="P151" s="58"/>
-      <c r="Q151" s="58"/>
-      <c r="R151" s="58"/>
-      <c r="S151" s="59"/>
+      <c r="C151" s="65"/>
+      <c r="D151" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="E151" s="66"/>
+      <c r="F151" s="66"/>
+      <c r="G151" s="66"/>
+      <c r="H151" s="66"/>
+      <c r="I151" s="66"/>
+      <c r="J151" s="66"/>
+      <c r="K151" s="66"/>
+      <c r="L151" s="66"/>
+      <c r="M151" s="66"/>
+      <c r="N151" s="66"/>
+      <c r="O151" s="66"/>
+      <c r="P151" s="66"/>
+      <c r="Q151" s="66"/>
+      <c r="R151" s="66"/>
+      <c r="S151" s="67"/>
     </row>
     <row r="154" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A154" s="30"/>
-      <c r="B154" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="C154" s="78"/>
-      <c r="D154" s="78"/>
-      <c r="E154" s="78"/>
-      <c r="F154" s="78"/>
-      <c r="G154" s="78"/>
-      <c r="H154" s="78"/>
-      <c r="I154" s="78"/>
-      <c r="J154" s="78"/>
-      <c r="K154" s="78"/>
-      <c r="L154" s="78"/>
-      <c r="M154" s="78"/>
-      <c r="N154" s="78"/>
-      <c r="O154" s="78"/>
-      <c r="P154" s="78"/>
-      <c r="Q154" s="78"/>
-      <c r="R154" s="78"/>
-      <c r="S154" s="78"/>
-      <c r="T154" s="78"/>
-      <c r="U154" s="78"/>
-      <c r="V154" s="78"/>
-      <c r="W154" s="78"/>
-      <c r="X154" s="78"/>
-      <c r="Y154" s="78"/>
+      <c r="B154" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C154" s="75"/>
+      <c r="D154" s="75"/>
+      <c r="E154" s="75"/>
+      <c r="F154" s="75"/>
+      <c r="G154" s="75"/>
+      <c r="H154" s="75"/>
+      <c r="I154" s="75"/>
+      <c r="J154" s="75"/>
+      <c r="K154" s="75"/>
+      <c r="L154" s="75"/>
+      <c r="M154" s="75"/>
+      <c r="N154" s="75"/>
+      <c r="O154" s="75"/>
+      <c r="P154" s="75"/>
+      <c r="Q154" s="75"/>
+      <c r="R154" s="75"/>
+      <c r="S154" s="75"/>
+      <c r="T154" s="75"/>
+      <c r="U154" s="75"/>
+      <c r="V154" s="75"/>
+      <c r="W154" s="75"/>
+      <c r="X154" s="75"/>
+      <c r="Y154" s="75"/>
     </row>
     <row r="156" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="77" t="s">
+      <c r="B156" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C156" s="77"/>
-      <c r="D156" s="77"/>
-      <c r="E156" s="77"/>
-      <c r="F156" s="77"/>
-      <c r="G156" s="77"/>
-      <c r="H156" s="77"/>
-      <c r="I156" s="77"/>
-      <c r="J156" s="77"/>
-      <c r="K156" s="77"/>
-      <c r="L156" s="77"/>
-      <c r="M156" s="77"/>
-      <c r="N156" s="77"/>
-      <c r="P156" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q156" s="60"/>
-      <c r="R156" s="60"/>
-      <c r="S156" s="60"/>
-      <c r="T156" s="60"/>
-      <c r="U156" s="60"/>
-      <c r="V156" s="60"/>
-      <c r="W156" s="60"/>
-      <c r="X156" s="60"/>
+      <c r="C156" s="78"/>
+      <c r="D156" s="78"/>
+      <c r="E156" s="78"/>
+      <c r="F156" s="78"/>
+      <c r="G156" s="78"/>
+      <c r="H156" s="78"/>
+      <c r="I156" s="78"/>
+      <c r="J156" s="78"/>
+      <c r="K156" s="78"/>
+      <c r="L156" s="78"/>
+      <c r="M156" s="78"/>
+      <c r="N156" s="78"/>
+      <c r="P156" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q156" s="79"/>
+      <c r="R156" s="79"/>
+      <c r="S156" s="79"/>
+      <c r="T156" s="79"/>
+      <c r="U156" s="79"/>
+      <c r="V156" s="79"/>
+      <c r="W156" s="79"/>
+      <c r="X156" s="79"/>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B157" s="9" t="s">
@@ -8134,46 +8199,46 @@
     </row>
     <row r="158" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B158" s="15"/>
-      <c r="C158" s="61" t="s">
+      <c r="C158" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D158" s="61"/>
-      <c r="E158" s="61"/>
-      <c r="F158" s="61"/>
-      <c r="G158" s="61"/>
-      <c r="H158" s="61"/>
-      <c r="I158" s="61"/>
-      <c r="J158" s="62"/>
-      <c r="K158" s="79" t="s">
+      <c r="D158" s="58"/>
+      <c r="E158" s="58"/>
+      <c r="F158" s="58"/>
+      <c r="G158" s="58"/>
+      <c r="H158" s="58"/>
+      <c r="I158" s="58"/>
+      <c r="J158" s="59"/>
+      <c r="K158" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="L158" s="80"/>
-      <c r="M158" s="80"/>
-      <c r="N158" s="81"/>
+      <c r="L158" s="84"/>
+      <c r="M158" s="84"/>
+      <c r="N158" s="85"/>
       <c r="P158" s="15"/>
-      <c r="Q158" s="61" t="s">
+      <c r="Q158" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="R158" s="61"/>
-      <c r="S158" s="61"/>
-      <c r="T158" s="61"/>
-      <c r="U158" s="61"/>
-      <c r="V158" s="61"/>
-      <c r="W158" s="61"/>
-      <c r="X158" s="62"/>
+      <c r="R158" s="58"/>
+      <c r="S158" s="58"/>
+      <c r="T158" s="58"/>
+      <c r="U158" s="58"/>
+      <c r="V158" s="58"/>
+      <c r="W158" s="58"/>
+      <c r="X158" s="59"/>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B159" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C159" s="63" t="s">
+      <c r="C159" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D159" s="64"/>
-      <c r="E159" s="65" t="s">
+      <c r="D159" s="61"/>
+      <c r="E159" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F159" s="65"/>
+      <c r="F159" s="56"/>
       <c r="G159" s="20" t="s">
         <v>23</v>
       </c>
@@ -8186,23 +8251,23 @@
       <c r="J159" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="K159" s="82" t="s">
-        <v>127</v>
-      </c>
-      <c r="L159" s="83"/>
-      <c r="M159" s="83"/>
-      <c r="N159" s="84"/>
+      <c r="K159" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="L159" s="80"/>
+      <c r="M159" s="80"/>
+      <c r="N159" s="118"/>
       <c r="P159" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q159" s="63" t="s">
+      <c r="Q159" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="R159" s="64"/>
-      <c r="S159" s="65" t="s">
+      <c r="R159" s="61"/>
+      <c r="S159" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="T159" s="65"/>
+      <c r="T159" s="56"/>
       <c r="U159" s="20" t="s">
         <v>23</v>
       </c>
@@ -8236,7 +8301,7 @@
         <v>42</v>
       </c>
       <c r="H160" s="24" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="I160" s="19" t="s">
         <v>39</v>
@@ -8245,16 +8310,16 @@
         <v>35</v>
       </c>
       <c r="K160" s="38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L160" s="33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M160" s="33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N160" s="39" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P160" s="12" t="s">
         <v>17</v>
@@ -8275,21 +8340,21 @@
         <v>42</v>
       </c>
       <c r="V160" s="24" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="W160" s="19" t="s">
         <v>41</v>
       </c>
       <c r="X160" s="37" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="161" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="162" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B162" s="66" t="s">
+      <c r="B162" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C162" s="67"/>
+      <c r="C162" s="77"/>
       <c r="D162" s="68" t="s">
         <v>4</v>
       </c>
@@ -8315,7 +8380,7 @@
       </c>
       <c r="C163" s="71"/>
       <c r="D163" s="72" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E163" s="73"/>
       <c r="F163" s="73"/>
@@ -8334,12 +8399,12 @@
       <c r="S163" s="74"/>
     </row>
     <row r="164" spans="2:19" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="75" t="s">
-        <v>127</v>
-      </c>
-      <c r="C164" s="76"/>
+      <c r="B164" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="C164" s="116"/>
       <c r="D164" s="72" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E164" s="73"/>
       <c r="F164" s="73"/>
@@ -8359,10 +8424,10 @@
     </row>
     <row r="165" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="166" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B166" s="66" t="s">
+      <c r="B166" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C166" s="67"/>
+      <c r="C166" s="77"/>
       <c r="D166" s="68" t="s">
         <v>4</v>
       </c>
@@ -8388,7 +8453,7 @@
       </c>
       <c r="C167" s="71"/>
       <c r="D167" s="72" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E167" s="73"/>
       <c r="F167" s="73"/>
@@ -8407,68 +8472,147 @@
       <c r="S167" s="74"/>
     </row>
     <row r="168" spans="2:19" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="56" t="s">
+      <c r="B168" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C168" s="57"/>
-      <c r="D168" s="58" t="s">
-        <v>140</v>
-      </c>
-      <c r="E168" s="58"/>
-      <c r="F168" s="58"/>
-      <c r="G168" s="58"/>
-      <c r="H168" s="58"/>
-      <c r="I168" s="58"/>
-      <c r="J168" s="58"/>
-      <c r="K168" s="58"/>
-      <c r="L168" s="58"/>
-      <c r="M168" s="58"/>
-      <c r="N168" s="58"/>
-      <c r="O168" s="58"/>
-      <c r="P168" s="58"/>
-      <c r="Q168" s="58"/>
-      <c r="R168" s="58"/>
-      <c r="S168" s="59"/>
+      <c r="C168" s="65"/>
+      <c r="D168" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="E168" s="66"/>
+      <c r="F168" s="66"/>
+      <c r="G168" s="66"/>
+      <c r="H168" s="66"/>
+      <c r="I168" s="66"/>
+      <c r="J168" s="66"/>
+      <c r="K168" s="66"/>
+      <c r="L168" s="66"/>
+      <c r="M168" s="66"/>
+      <c r="N168" s="66"/>
+      <c r="O168" s="66"/>
+      <c r="P168" s="66"/>
+      <c r="Q168" s="66"/>
+      <c r="R168" s="66"/>
+      <c r="S168" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="198">
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="O73:P73"/>
-    <mergeCell ref="O79:P79"/>
-    <mergeCell ref="Y73:Z73"/>
-    <mergeCell ref="Y79:Z79"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="O109:P109"/>
-    <mergeCell ref="Y109:Z109"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="V39:AD39"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:S65"/>
-    <mergeCell ref="D124:S124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="D125:S125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="D126:S126"/>
-    <mergeCell ref="B104:Y104"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="D137:S137"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="B117:Y117"/>
-    <mergeCell ref="C120:J120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="B129:Y129"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="C108:J108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="V106:AD106"/>
-    <mergeCell ref="W108:AD108"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="D168:S168"/>
+    <mergeCell ref="P156:X156"/>
+    <mergeCell ref="Q158:X158"/>
+    <mergeCell ref="Q159:R159"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:S162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="D163:S163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="D164:S164"/>
+    <mergeCell ref="B156:N156"/>
+    <mergeCell ref="B154:Y154"/>
+    <mergeCell ref="C158:J158"/>
+    <mergeCell ref="K158:N158"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="K159:N159"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="D166:S166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="D167:S167"/>
+    <mergeCell ref="E159:F159"/>
+    <mergeCell ref="S159:T159"/>
+    <mergeCell ref="B142:Y142"/>
+    <mergeCell ref="C145:J145"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="D149:S149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:S150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="D151:S151"/>
+    <mergeCell ref="E146:F146"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:S97"/>
+    <mergeCell ref="V131:AD131"/>
+    <mergeCell ref="W133:AD133"/>
+    <mergeCell ref="W134:X134"/>
+    <mergeCell ref="L106:T106"/>
+    <mergeCell ref="M108:T108"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="L131:T131"/>
+    <mergeCell ref="M133:T133"/>
+    <mergeCell ref="M134:N134"/>
+    <mergeCell ref="W109:X109"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="O134:P134"/>
+    <mergeCell ref="Y134:Z134"/>
+    <mergeCell ref="D61:S61"/>
+    <mergeCell ref="D60:S60"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D59:S59"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="D95:S95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:S96"/>
+    <mergeCell ref="B88:Y88"/>
+    <mergeCell ref="C91:J91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="B70:J70"/>
+    <mergeCell ref="C72:J72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="L70:T70"/>
+    <mergeCell ref="M72:T72"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="B68:Y68"/>
+    <mergeCell ref="V70:AD70"/>
+    <mergeCell ref="W72:AD72"/>
+    <mergeCell ref="W73:X73"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:S57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:S58"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:S32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:S33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B50:Y50"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="D34:S34"/>
+    <mergeCell ref="B37:Y37"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="S54:V54"/>
+    <mergeCell ref="K53:V53"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B2:Y2"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="B8:Y8"/>
+    <mergeCell ref="B24:Y24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:J15"/>
     <mergeCell ref="B138:C138"/>
     <mergeCell ref="D138:S138"/>
     <mergeCell ref="B83:C83"/>
@@ -8493,6 +8637,34 @@
     <mergeCell ref="D101:S101"/>
     <mergeCell ref="B131:J131"/>
     <mergeCell ref="C133:J133"/>
+    <mergeCell ref="D124:S124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="D125:S125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="D126:S126"/>
+    <mergeCell ref="B104:Y104"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="D137:S137"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="B117:Y117"/>
+    <mergeCell ref="C120:J120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="B129:Y129"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="C108:J108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="V106:AD106"/>
+    <mergeCell ref="W108:AD108"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="V39:AD39"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:S65"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="D63:S63"/>
     <mergeCell ref="B64:C64"/>
@@ -8508,128 +8680,21 @@
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="D47:S47"/>
     <mergeCell ref="O54:R54"/>
-    <mergeCell ref="S54:V54"/>
-    <mergeCell ref="K53:V53"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B2:Y2"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="B8:Y8"/>
-    <mergeCell ref="B24:Y24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:S57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:S58"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:S32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:S33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B50:Y50"/>
-    <mergeCell ref="C53:J53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="D34:S34"/>
-    <mergeCell ref="B37:Y37"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="D61:S61"/>
-    <mergeCell ref="D60:S60"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D59:S59"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="D95:S95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:S96"/>
-    <mergeCell ref="B88:Y88"/>
-    <mergeCell ref="C91:J91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="B70:J70"/>
-    <mergeCell ref="C72:J72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="L70:T70"/>
-    <mergeCell ref="M72:T72"/>
-    <mergeCell ref="M73:N73"/>
-    <mergeCell ref="B68:Y68"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:S97"/>
-    <mergeCell ref="V131:AD131"/>
-    <mergeCell ref="W133:AD133"/>
-    <mergeCell ref="W134:X134"/>
-    <mergeCell ref="L106:T106"/>
-    <mergeCell ref="M108:T108"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="L131:T131"/>
-    <mergeCell ref="M133:T133"/>
-    <mergeCell ref="M134:N134"/>
-    <mergeCell ref="W109:X109"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E134:F134"/>
-    <mergeCell ref="O134:P134"/>
-    <mergeCell ref="Y134:Z134"/>
-    <mergeCell ref="V70:AD70"/>
-    <mergeCell ref="W72:AD72"/>
-    <mergeCell ref="W73:X73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="O73:P73"/>
+    <mergeCell ref="O79:P79"/>
+    <mergeCell ref="Y73:Z73"/>
+    <mergeCell ref="Y79:Z79"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="O109:P109"/>
+    <mergeCell ref="Y109:Z109"/>
     <mergeCell ref="L76:T76"/>
     <mergeCell ref="M78:T78"/>
     <mergeCell ref="M79:N79"/>
     <mergeCell ref="V76:AD76"/>
     <mergeCell ref="W78:AD78"/>
     <mergeCell ref="W79:X79"/>
-    <mergeCell ref="B142:Y142"/>
-    <mergeCell ref="C145:J145"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="D149:S149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="D150:S150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="D151:S151"/>
-    <mergeCell ref="E146:F146"/>
-    <mergeCell ref="B154:Y154"/>
-    <mergeCell ref="C158:J158"/>
-    <mergeCell ref="K158:N158"/>
-    <mergeCell ref="C159:D159"/>
-    <mergeCell ref="K159:N159"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="D166:S166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="D167:S167"/>
-    <mergeCell ref="E159:F159"/>
-    <mergeCell ref="S159:T159"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="D168:S168"/>
-    <mergeCell ref="P156:X156"/>
-    <mergeCell ref="Q158:X158"/>
-    <mergeCell ref="Q159:R159"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="D162:S162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="D163:S163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="D164:S164"/>
-    <mergeCell ref="B156:N156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>